<commit_message>
Portfolio metadata sheet added
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio - Current Projects 1.29.2024.xlsx
+++ b/data/SJV Portfolio - Current Projects 1.29.2024.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/Portfolio Inventory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904F5342-100F-9C43-A34F-0C041CF59FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296891D8-8D48-0742-9611-35D6DF175F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="880" windowWidth="34000" windowHeight="20800" activeTab="1" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
+    <workbookView xWindow="560" yWindow="880" windowWidth="34000" windowHeight="20800" activeTab="4" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="feedstock_to_commodity" sheetId="3" r:id="rId2"/>
-    <sheet name="commodity_to_use" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="portfolio_input" sheetId="1" r:id="rId1"/>
+    <sheet name="portfolio_metadata" sheetId="6" r:id="rId2"/>
+    <sheet name="feedstock_to_commodity" sheetId="3" r:id="rId3"/>
+    <sheet name="commodity_to_use" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="103">
   <si>
     <t>Solar</t>
   </si>
@@ -260,9 +261,6 @@
     <t>Hydrogen Use</t>
   </si>
   <si>
-    <t>Name: Current Projects Portfolio</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -302,115 +300,139 @@
     <t>Step 1: Name and Describe Your Portfolio</t>
   </si>
   <si>
-    <t>Description: This portfolio describes The Current Projects portfolio reflects clean energy development projects that are being planned for or under way in the SJV. This includes:
+    <t>Step 3: What percent of the produced hydrogen should go to transportation vs. ammonia</t>
+  </si>
+  <si>
+    <t>Feedstock</t>
+  </si>
+  <si>
+    <t>“Primary” Conversion Technology</t>
+  </si>
+  <si>
+    <t>Commodity</t>
+  </si>
+  <si>
+    <t>Commodity Unit</t>
+  </si>
+  <si>
+    <t>Unit Code</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>Megawatts</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Wind turbine</t>
+  </si>
+  <si>
+    <t>Battery Storage</t>
+  </si>
+  <si>
+    <t>Pumped hydro</t>
+  </si>
+  <si>
+    <t>Gasification + Gas Engine</t>
+  </si>
+  <si>
+    <t>PV + Electrolysis</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>SMR + CCS</t>
+  </si>
+  <si>
+    <t>Gasification/ Pyrolysis + Conditioning</t>
+  </si>
+  <si>
+    <t>Anaerobic Digestion + Conditioning</t>
+  </si>
+  <si>
+    <t>MCF</t>
+  </si>
+  <si>
+    <t>HEFA</t>
+  </si>
+  <si>
+    <t>MGal</t>
+  </si>
+  <si>
+    <t>FT-Gasification</t>
+  </si>
+  <si>
+    <t>Input Category</t>
+  </si>
+  <si>
+    <t>Solar/Wind</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Biomass</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>Power Grid</t>
+  </si>
+  <si>
+    <t>Surface Transport Fuel</t>
+  </si>
+  <si>
+    <t>Ammonia Production</t>
+  </si>
+  <si>
+    <t>Gas Grid</t>
+  </si>
+  <si>
+    <t>Aviation Fuel</t>
+  </si>
+  <si>
+    <t>Anaerobic Digestion + Conditioning + Gas Engine</t>
+  </si>
+  <si>
+    <t>Anaerobic Digestion + SMR or ATR (Autothermal Reforming)</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Metadata Value</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Creator</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Current Projects Portfolio</t>
+  </si>
+  <si>
+    <t>This portfolio describes The Current Projects portfolio reflects clean energy development projects that are being planned for or under way in the SJV. This includes:
 • Anticipated electricity resource buildouts described in the IPR Busbar Study (cite) that are associated with substations located in the SJV. This includes a buildout of 13.3 GW of utility solar, 270 MW of wind, 20MW of biomass and biomethane, 7.4 GW of battery storage, and 1 GW of long-duration energy storage. We allocate biomass and biogas to feedstocks according to the relative electricity production potential of each resource, as shown in Table B.2.
 • The Lone Cypress Blue Hydrogen facility located in Kern County and scheduled to come online in 2026 and produce 30 tons of H2 per day (11,000 tons/year) (California Resources Corporation, undated)
 • The DOE Hydrogen Hub facilities located in the Central Valley. The DOE has indicated that a total of 3 MMT of hydrogen will be produced from the 7 facilities. We estimate that the SJV would produce approximately 215,000 tons of hydrogen per year, if California produced 1/7th of the DOE total, and if half of California’s production took place in the SJV as suggested by the proposed facility locations (cite). The production of hydrogen by resource type is not available for these facilities. Connelly et al. (2020) suggest that solar production potential in the SJV may be 10 times larger than biogas production potential, which may be 10 times larger than biomass production potential. Consistent with this, we assume approximately 90% of production from solar, and 9% from biomethane, and 1% from biomass. We allocate biomass and biogas to feedstocks according to the relative hydrogen production potential of each resource.</t>
   </si>
   <si>
-    <t>Step 3: What percent of the produced hydrogen should go to transportation vs. ammonia</t>
-  </si>
-  <si>
-    <t>Feedstock</t>
-  </si>
-  <si>
-    <t>“Primary” Conversion Technology</t>
-  </si>
-  <si>
-    <t>Commodity</t>
-  </si>
-  <si>
-    <t>Commodity Unit</t>
-  </si>
-  <si>
-    <t>Unit Code</t>
-  </si>
-  <si>
-    <t>PV</t>
-  </si>
-  <si>
-    <t>Megawatts</t>
-  </si>
-  <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>Wind turbine</t>
-  </si>
-  <si>
-    <t>Battery Storage</t>
-  </si>
-  <si>
-    <t>Pumped hydro</t>
-  </si>
-  <si>
-    <t>Gasification + Gas Engine</t>
-  </si>
-  <si>
-    <t>PV + Electrolysis</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>SMR + CCS</t>
-  </si>
-  <si>
-    <t>Gasification/ Pyrolysis + Conditioning</t>
-  </si>
-  <si>
-    <t>Anaerobic Digestion + Conditioning</t>
-  </si>
-  <si>
-    <t>MCF</t>
-  </si>
-  <si>
-    <t>HEFA</t>
-  </si>
-  <si>
-    <t>MGal</t>
-  </si>
-  <si>
-    <t>FT-Gasification</t>
-  </si>
-  <si>
-    <t>Input Category</t>
-  </si>
-  <si>
-    <t>Solar/Wind</t>
-  </si>
-  <si>
-    <t>Storage</t>
-  </si>
-  <si>
-    <t>Biomass</t>
-  </si>
-  <si>
-    <t>Natural Gas</t>
-  </si>
-  <si>
-    <t>Use</t>
-  </si>
-  <si>
-    <t>Power Grid</t>
-  </si>
-  <si>
-    <t>Surface Transport Fuel</t>
-  </si>
-  <si>
-    <t>Ammonia Production</t>
-  </si>
-  <si>
-    <t>Gas Grid</t>
-  </si>
-  <si>
-    <t>Aviation Fuel</t>
-  </si>
-  <si>
-    <t>Anaerobic Digestion + Conditioning + Gas Engine</t>
-  </si>
-  <si>
-    <t>Anaerobic Digestion + SMR or ATR (Autothermal Reforming)</t>
+    <t>Nidhi Kalra (nidhi@rand.org)</t>
   </si>
 </sst>
 </file>
@@ -559,7 +581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -607,6 +629,19 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -616,19 +651,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA35989-F8F5-C645-8F8C-CB2D79A95BD0}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="133" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -984,39 +1009,42 @@
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:7" ht="115" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-    </row>
-    <row r="4" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -1024,12 +1052,12 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1049,7 +1077,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1069,7 +1097,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1089,7 +1117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1109,7 +1137,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1129,7 +1157,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1149,7 +1177,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1169,7 +1197,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1181,7 +1209,7 @@
       </c>
       <c r="D14" s="14"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1193,7 +1221,7 @@
       </c>
       <c r="D15" s="14"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1408,7 +1436,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1463,10 +1491,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BDCA78-19E5-1044-A930-DF4D7DAFD93C}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="33" t="str">
+        <f>portfolio_input!B3</f>
+        <v>Current Projects Portfolio</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="str">
+        <f>portfolio_input!G3</f>
+        <v>Nidhi Kalra (nidhi@rand.org)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="34">
+        <v>45322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="33" t="str">
+        <f>portfolio_input!D3</f>
+        <v>This portfolio describes The Current Projects portfolio reflects clean energy development projects that are being planned for or under way in the SJV. This includes:
+• Anticipated electricity resource buildouts described in the IPR Busbar Study (cite) that are associated with substations located in the SJV. This includes a buildout of 13.3 GW of utility solar, 270 MW of wind, 20MW of biomass and biomethane, 7.4 GW of battery storage, and 1 GW of long-duration energy storage. We allocate biomass and biogas to feedstocks according to the relative electricity production potential of each resource, as shown in Table B.2.
+• The Lone Cypress Blue Hydrogen facility located in Kern County and scheduled to come online in 2026 and produce 30 tons of H2 per day (11,000 tons/year) (California Resources Corporation, undated)
+• The DOE Hydrogen Hub facilities located in the Central Valley. The DOE has indicated that a total of 3 MMT of hydrogen will be produced from the 7 facilities. We estimate that the SJV would produce approximately 215,000 tons of hydrogen per year, if California produced 1/7th of the DOE total, and if half of California’s production took place in the SJV as suggested by the proposed facility locations (cite). The production of hydrogen by resource type is not available for these facilities. Connelly et al. (2020) suggest that solar production potential in the SJV may be 10 times larger than biogas production potential, which may be 10 times larger than biomass production potential. Consistent with this, we assume approximately 90% of production from solar, and 9% from biomethane, and 1% from biomass. We allocate biomass and biogas to feedstocks according to the relative hydrogen production potential of each resource.</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225537EC-F8DB-7B4E-B90C-2D6AA935C6A7}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -1480,22 +1572,22 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>66</v>
       </c>
       <c r="G1">
         <v>2025</v>
@@ -1563,22 +1655,22 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" t="s">
-        <v>69</v>
       </c>
       <c r="G2">
         <f>$Q2/11</f>
@@ -1621,7 +1713,7 @@
         <v>12090.909090909088</v>
       </c>
       <c r="Q2">
-        <f>Sheet1!C8*1000</f>
+        <f>portfolio_input!C8*1000</f>
         <v>13300</v>
       </c>
       <c r="R2">
@@ -1667,22 +1759,22 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G15" si="2">$Q3/11</f>
@@ -1725,7 +1817,7 @@
         <v>245.4545454545455</v>
       </c>
       <c r="Q3">
-        <f>Sheet1!C9*1000</f>
+        <f>portfolio_input!C9*1000</f>
         <v>270</v>
       </c>
       <c r="R3">
@@ -1771,22 +1863,22 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
@@ -1829,7 +1921,7 @@
         <v>6727.2727272727288</v>
       </c>
       <c r="Q4">
-        <f>Sheet1!C10*1000</f>
+        <f>portfolio_input!C10*1000</f>
         <v>7400</v>
       </c>
       <c r="R4">
@@ -1875,22 +1967,22 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
@@ -1933,7 +2025,7 @@
         <v>909.09090909090889</v>
       </c>
       <c r="Q5">
-        <f>Sheet1!C11*1000</f>
+        <f>portfolio_input!C11*1000</f>
         <v>1000</v>
       </c>
       <c r="R5">
@@ -1979,22 +2071,22 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
@@ -2037,7 +2129,7 @@
         <v>9.5990965556182957</v>
       </c>
       <c r="Q6">
-        <f>Sheet1!C12*1000</f>
+        <f>portfolio_input!C12*1000</f>
         <v>10.559006211180124</v>
       </c>
       <c r="R6">
@@ -2083,22 +2175,22 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
@@ -2141,7 +2233,7 @@
         <v>1.5810276679841897</v>
       </c>
       <c r="Q7">
-        <f>Sheet1!C13*1000</f>
+        <f>portfolio_input!C13*1000</f>
         <v>1.7391304347826089</v>
       </c>
       <c r="R7">
@@ -2187,22 +2279,22 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
@@ -2245,7 +2337,7 @@
         <v>6.7758328627893851</v>
       </c>
       <c r="Q8">
-        <f>Sheet1!C14*1000</f>
+        <f>portfolio_input!C14*1000</f>
         <v>7.4534161490683237</v>
       </c>
       <c r="R8">
@@ -2291,22 +2383,22 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
@@ -2349,7 +2441,7 @@
         <v>0.22586109542631283</v>
       </c>
       <c r="Q9">
-        <f>Sheet1!C15*1000</f>
+        <f>portfolio_input!C15*1000</f>
         <v>0.2484472049689441</v>
       </c>
       <c r="R9">
@@ -2395,13 +2487,13 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -2410,7 +2502,7 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
@@ -2452,7 +2544,7 @@
         <f t="shared" si="3"/>
         <v>175909.09090909091</v>
       </c>
-      <c r="Q10" s="29">
+      <c r="Q10" s="26">
         <f>215000*0.9</f>
         <v>193500</v>
       </c>
@@ -2499,13 +2591,13 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -2514,7 +2606,7 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
@@ -2556,7 +2648,7 @@
         <f t="shared" si="3"/>
         <v>10000</v>
       </c>
-      <c r="Q11" s="30">
+      <c r="Q11" s="27">
         <v>11000</v>
       </c>
       <c r="R11">
@@ -2602,13 +2694,13 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -2617,7 +2709,7 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
@@ -2659,7 +2751,7 @@
         <f t="shared" si="3"/>
         <v>9750</v>
       </c>
-      <c r="Q12" s="32">
+      <c r="Q12" s="29">
         <v>10725</v>
       </c>
       <c r="R12">
@@ -2705,13 +2797,13 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -2720,7 +2812,7 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
@@ -2762,7 +2854,7 @@
         <f t="shared" si="3"/>
         <v>1610</v>
       </c>
-      <c r="Q13" s="32">
+      <c r="Q13" s="29">
         <v>1771</v>
       </c>
       <c r="R13">
@@ -2808,13 +2900,13 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
@@ -2823,7 +2915,7 @@
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
@@ -2865,8 +2957,8 @@
         <f t="shared" si="3"/>
         <v>7709.090909090909</v>
       </c>
-      <c r="Q14" s="32">
-        <f>Sheet1!C20</f>
+      <c r="Q14" s="29">
+        <f>portfolio_input!C20</f>
         <v>8480</v>
       </c>
       <c r="R14">
@@ -2912,13 +3004,13 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -2927,7 +3019,7 @@
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
@@ -2969,8 +3061,8 @@
         <f t="shared" si="3"/>
         <v>491.81818181818181</v>
       </c>
-      <c r="Q15" s="32">
-        <f>Sheet1!C21</f>
+      <c r="Q15" s="29">
+        <f>portfolio_input!C21</f>
         <v>541</v>
       </c>
       <c r="R15">
@@ -3016,13 +3108,13 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -3031,19 +3123,19 @@
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q16" s="31"/>
+        <v>77</v>
+      </c>
+      <c r="Q16" s="28"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -3052,18 +3144,18 @@
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
@@ -3072,18 +3164,18 @@
         <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -3092,18 +3184,18 @@
         <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -3112,7 +3204,7 @@
         <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -3120,7 +3212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A302D73-9F74-D647-9FC8-5951743D164F}">
   <dimension ref="A1:W6"/>
   <sheetViews>
@@ -3135,428 +3227,428 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="25">
+        <v>2025</v>
+      </c>
+      <c r="D1" s="25">
+        <v>2026</v>
+      </c>
+      <c r="E1" s="25">
+        <v>2027</v>
+      </c>
+      <c r="F1" s="25">
+        <v>2028</v>
+      </c>
+      <c r="G1" s="25">
+        <v>2029</v>
+      </c>
+      <c r="H1" s="25">
+        <v>2030</v>
+      </c>
+      <c r="I1" s="25">
+        <v>2031</v>
+      </c>
+      <c r="J1" s="25">
+        <v>2032</v>
+      </c>
+      <c r="K1" s="25">
+        <v>2033</v>
+      </c>
+      <c r="L1" s="25">
+        <v>2034</v>
+      </c>
+      <c r="M1" s="25">
+        <v>2035</v>
+      </c>
+      <c r="N1" s="25">
+        <v>2036</v>
+      </c>
+      <c r="O1" s="25">
+        <v>2037</v>
+      </c>
+      <c r="P1" s="25">
+        <v>2038</v>
+      </c>
+      <c r="Q1" s="25">
+        <v>2039</v>
+      </c>
+      <c r="R1" s="25">
+        <v>2040</v>
+      </c>
+      <c r="S1" s="25">
+        <v>2041</v>
+      </c>
+      <c r="T1" s="25">
+        <v>2042</v>
+      </c>
+      <c r="U1" s="25">
+        <v>2043</v>
+      </c>
+      <c r="V1" s="25">
+        <v>2044</v>
+      </c>
+      <c r="W1" s="25">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="25">
+        <v>1</v>
+      </c>
+      <c r="D2" s="25">
+        <v>1</v>
+      </c>
+      <c r="E2" s="25">
+        <v>1</v>
+      </c>
+      <c r="F2" s="25">
+        <v>1</v>
+      </c>
+      <c r="G2" s="25">
+        <v>1</v>
+      </c>
+      <c r="H2" s="25">
+        <v>1</v>
+      </c>
+      <c r="I2" s="25">
+        <v>1</v>
+      </c>
+      <c r="J2" s="25">
+        <v>1</v>
+      </c>
+      <c r="K2" s="25">
+        <v>1</v>
+      </c>
+      <c r="L2" s="25">
+        <v>1</v>
+      </c>
+      <c r="M2" s="25">
+        <v>1</v>
+      </c>
+      <c r="N2" s="25">
+        <v>1</v>
+      </c>
+      <c r="O2" s="25">
+        <v>1</v>
+      </c>
+      <c r="P2" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="25">
+        <v>1</v>
+      </c>
+      <c r="R2" s="25">
+        <v>1</v>
+      </c>
+      <c r="S2" s="25">
+        <v>1</v>
+      </c>
+      <c r="T2" s="25">
+        <v>1</v>
+      </c>
+      <c r="U2" s="25">
+        <v>1</v>
+      </c>
+      <c r="V2" s="25">
+        <v>1</v>
+      </c>
+      <c r="W2" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="28">
-        <v>2025</v>
-      </c>
-      <c r="D1" s="28">
-        <v>2026</v>
-      </c>
-      <c r="E1" s="28">
-        <v>2027</v>
-      </c>
-      <c r="F1" s="28">
-        <v>2028</v>
-      </c>
-      <c r="G1" s="28">
-        <v>2029</v>
-      </c>
-      <c r="H1" s="28">
-        <v>2030</v>
-      </c>
-      <c r="I1" s="28">
-        <v>2031</v>
-      </c>
-      <c r="J1" s="28">
-        <v>2032</v>
-      </c>
-      <c r="K1" s="28">
-        <v>2033</v>
-      </c>
-      <c r="L1" s="28">
-        <v>2034</v>
-      </c>
-      <c r="M1" s="28">
-        <v>2035</v>
-      </c>
-      <c r="N1" s="28">
-        <v>2036</v>
-      </c>
-      <c r="O1" s="28">
-        <v>2037</v>
-      </c>
-      <c r="P1" s="28">
-        <v>2038</v>
-      </c>
-      <c r="Q1" s="28">
-        <v>2039</v>
-      </c>
-      <c r="R1" s="28">
-        <v>2040</v>
-      </c>
-      <c r="S1" s="28">
-        <v>2041</v>
-      </c>
-      <c r="T1" s="28">
-        <v>2042</v>
-      </c>
-      <c r="U1" s="28">
-        <v>2043</v>
-      </c>
-      <c r="V1" s="28">
-        <v>2044</v>
-      </c>
-      <c r="W1" s="28">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="28" t="s">
+      <c r="C3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="N3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="P3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="R3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="S3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="T3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="U3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="V3" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="W3" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="28">
-        <v>1</v>
-      </c>
-      <c r="D2" s="28">
-        <v>1</v>
-      </c>
-      <c r="E2" s="28">
-        <v>1</v>
-      </c>
-      <c r="F2" s="28">
-        <v>1</v>
-      </c>
-      <c r="G2" s="28">
-        <v>1</v>
-      </c>
-      <c r="H2" s="28">
-        <v>1</v>
-      </c>
-      <c r="I2" s="28">
-        <v>1</v>
-      </c>
-      <c r="J2" s="28">
-        <v>1</v>
-      </c>
-      <c r="K2" s="28">
-        <v>1</v>
-      </c>
-      <c r="L2" s="28">
-        <v>1</v>
-      </c>
-      <c r="M2" s="28">
-        <v>1</v>
-      </c>
-      <c r="N2" s="28">
-        <v>1</v>
-      </c>
-      <c r="O2" s="28">
-        <v>1</v>
-      </c>
-      <c r="P2" s="28">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="28">
-        <v>1</v>
-      </c>
-      <c r="R2" s="28">
-        <v>1</v>
-      </c>
-      <c r="S2" s="28">
-        <v>1</v>
-      </c>
-      <c r="T2" s="28">
-        <v>1</v>
-      </c>
-      <c r="U2" s="28">
-        <v>1</v>
-      </c>
-      <c r="V2" s="28">
-        <v>1</v>
-      </c>
-      <c r="W2" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="28" t="s">
+      <c r="C4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="N4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="O4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="P4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Q4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="R4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="S4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="T4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="U4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="V4" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="W4" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="F3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="J3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="M3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="N3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="O3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="P3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="Q3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="R3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="S3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="T3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="U3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="V3" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="W3" s="28">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="28" t="s">
+      <c r="C5" s="25">
+        <v>1</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
+      <c r="E5" s="25">
+        <v>1</v>
+      </c>
+      <c r="F5" s="25">
+        <v>1</v>
+      </c>
+      <c r="G5" s="25">
+        <v>1</v>
+      </c>
+      <c r="H5" s="25">
+        <v>1</v>
+      </c>
+      <c r="I5" s="25">
+        <v>1</v>
+      </c>
+      <c r="J5" s="25">
+        <v>1</v>
+      </c>
+      <c r="K5" s="25">
+        <v>1</v>
+      </c>
+      <c r="L5" s="25">
+        <v>1</v>
+      </c>
+      <c r="M5" s="25">
+        <v>1</v>
+      </c>
+      <c r="N5" s="25">
+        <v>1</v>
+      </c>
+      <c r="O5" s="25">
+        <v>1</v>
+      </c>
+      <c r="P5" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="25">
+        <v>1</v>
+      </c>
+      <c r="R5" s="25">
+        <v>1</v>
+      </c>
+      <c r="S5" s="25">
+        <v>1</v>
+      </c>
+      <c r="T5" s="25">
+        <v>1</v>
+      </c>
+      <c r="U5" s="25">
+        <v>1</v>
+      </c>
+      <c r="V5" s="25">
+        <v>1</v>
+      </c>
+      <c r="W5" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="H4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="I4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="J4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="K4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="L4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="M4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="N4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="O4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="P4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="Q4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="R4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="S4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="T4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="U4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="V4" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="W4" s="28">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="28">
-        <v>1</v>
-      </c>
-      <c r="D5" s="28">
-        <v>1</v>
-      </c>
-      <c r="E5" s="28">
-        <v>1</v>
-      </c>
-      <c r="F5" s="28">
-        <v>1</v>
-      </c>
-      <c r="G5" s="28">
-        <v>1</v>
-      </c>
-      <c r="H5" s="28">
-        <v>1</v>
-      </c>
-      <c r="I5" s="28">
-        <v>1</v>
-      </c>
-      <c r="J5" s="28">
-        <v>1</v>
-      </c>
-      <c r="K5" s="28">
-        <v>1</v>
-      </c>
-      <c r="L5" s="28">
-        <v>1</v>
-      </c>
-      <c r="M5" s="28">
-        <v>1</v>
-      </c>
-      <c r="N5" s="28">
-        <v>1</v>
-      </c>
-      <c r="O5" s="28">
-        <v>1</v>
-      </c>
-      <c r="P5" s="28">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="28">
-        <v>1</v>
-      </c>
-      <c r="R5" s="28">
-        <v>1</v>
-      </c>
-      <c r="S5" s="28">
-        <v>1</v>
-      </c>
-      <c r="T5" s="28">
-        <v>1</v>
-      </c>
-      <c r="U5" s="28">
-        <v>1</v>
-      </c>
-      <c r="V5" s="28">
-        <v>1</v>
-      </c>
-      <c r="W5" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="28">
-        <v>1</v>
-      </c>
-      <c r="D6" s="28">
-        <v>1</v>
-      </c>
-      <c r="E6" s="28">
-        <v>1</v>
-      </c>
-      <c r="F6" s="28">
-        <v>1</v>
-      </c>
-      <c r="G6" s="28">
-        <v>1</v>
-      </c>
-      <c r="H6" s="28">
-        <v>1</v>
-      </c>
-      <c r="I6" s="28">
-        <v>1</v>
-      </c>
-      <c r="J6" s="28">
-        <v>1</v>
-      </c>
-      <c r="K6" s="28">
-        <v>1</v>
-      </c>
-      <c r="L6" s="28">
-        <v>1</v>
-      </c>
-      <c r="M6" s="28">
-        <v>1</v>
-      </c>
-      <c r="N6" s="28">
-        <v>1</v>
-      </c>
-      <c r="O6" s="28">
-        <v>1</v>
-      </c>
-      <c r="P6" s="28">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="28">
-        <v>1</v>
-      </c>
-      <c r="R6" s="28">
-        <v>1</v>
-      </c>
-      <c r="S6" s="28">
-        <v>1</v>
-      </c>
-      <c r="T6" s="28">
-        <v>1</v>
-      </c>
-      <c r="U6" s="28">
-        <v>1</v>
-      </c>
-      <c r="V6" s="28">
-        <v>1</v>
-      </c>
-      <c r="W6" s="28">
+      <c r="C6" s="25">
+        <v>1</v>
+      </c>
+      <c r="D6" s="25">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25">
+        <v>1</v>
+      </c>
+      <c r="F6" s="25">
+        <v>1</v>
+      </c>
+      <c r="G6" s="25">
+        <v>1</v>
+      </c>
+      <c r="H6" s="25">
+        <v>1</v>
+      </c>
+      <c r="I6" s="25">
+        <v>1</v>
+      </c>
+      <c r="J6" s="25">
+        <v>1</v>
+      </c>
+      <c r="K6" s="25">
+        <v>1</v>
+      </c>
+      <c r="L6" s="25">
+        <v>1</v>
+      </c>
+      <c r="M6" s="25">
+        <v>1</v>
+      </c>
+      <c r="N6" s="25">
+        <v>1</v>
+      </c>
+      <c r="O6" s="25">
+        <v>1</v>
+      </c>
+      <c r="P6" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="25">
+        <v>1</v>
+      </c>
+      <c r="R6" s="25">
+        <v>1</v>
+      </c>
+      <c r="S6" s="25">
+        <v>1</v>
+      </c>
+      <c r="T6" s="25">
+        <v>1</v>
+      </c>
+      <c r="U6" s="25">
+        <v>1</v>
+      </c>
+      <c r="V6" s="25">
+        <v>1</v>
+      </c>
+      <c r="W6" s="25">
         <v>1</v>
       </c>
     </row>
@@ -3565,12 +3657,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCD9FC6-402B-8D4F-AF23-A8506C6A96EC}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3581,24 +3673,24 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>55</v>
-      </c>
-      <c r="G1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="18">
         <v>654000</v>
@@ -3647,13 +3739,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>30</v>
@@ -3681,7 +3773,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>480</v>
@@ -3690,10 +3782,10 @@
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7">
         <v>13</v>
@@ -3722,7 +3814,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>0.85</v>
@@ -3771,7 +3863,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12">
         <v>0.02</v>
@@ -3795,7 +3887,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="5">
         <v>21500</v>

</xml_diff>

<commit_message>
Updated portfolios with methane->elec and methane->H2 removed
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio - Current Projects 1.29.2024.xlsx
+++ b/data/SJV Portfolio - Current Projects 1.29.2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50FBA73-EF2F-7A4F-96BA-40AF7678DA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F118EA7E-10F1-4E44-8A47-05F558FFB153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="880" windowWidth="34000" windowHeight="20800" activeTab="2" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
+    <workbookView xWindow="560" yWindow="880" windowWidth="34000" windowHeight="17980" activeTab="2" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
   </bookViews>
   <sheets>
     <sheet name="portfolio_input" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="97">
   <si>
     <t>Solar</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Diverted Organic Waste</t>
-  </si>
-  <si>
-    <t>Plant Oils</t>
   </si>
   <si>
     <t>Sustainable Aviation Fuel</t>
@@ -384,9 +381,6 @@
     <t>Aviation Fuel</t>
   </si>
   <si>
-    <t>Anaerobic Digestion + Conditioning + Gas Engine</t>
-  </si>
-  <si>
     <t>Anaerobic Digestion + SMR or ATR (Autothermal Reforming)</t>
   </si>
   <si>
@@ -415,6 +409,9 @@
   </si>
   <si>
     <t>This portfolio describes The Current Projects portfolio reflects clean energy development projects that are being planned for or under way in the SJV. THIS PORTFOLIO ONLY USES BIOGAS TO PRODUCE BIOMETHANE FOR THE GAS GRID WHILE WE UPDATE THE MODEL.</t>
+  </si>
+  <si>
+    <t>Anaerobic Digestion + Conditioning + Combustion</t>
   </si>
 </sst>
 </file>
@@ -563,7 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -605,20 +602,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -979,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA35989-F8F5-C645-8F8C-CB2D79A95BD0}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="133" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView topLeftCell="A6" zoomScale="133" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,37 +984,37 @@
   <sheetData>
     <row r="1" spans="1:7" s="8" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:7" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34" t="s">
+      <c r="A2" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="31" t="s">
-        <v>96</v>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="28" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
@@ -1039,27 +1027,27 @@
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="F7" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1076,10 +1064,10 @@
         <v>26.6</v>
       </c>
       <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
         <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1096,10 +1084,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1116,10 +1104,10 @@
         <v>14.8</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1136,10 +1124,10 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1149,17 +1137,17 @@
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="32">
-        <v>1.7171717171717171E-2</v>
+      <c r="C12" s="29">
+        <v>1.0559006211180125E-2</v>
       </c>
       <c r="D12" s="14">
         <v>0.02</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1169,17 +1157,17 @@
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="32">
-        <v>2.8282828282828287E-3</v>
+      <c r="C13" s="29">
+        <v>1.739130434782609E-3</v>
       </c>
       <c r="D13" s="13">
         <v>0.02</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1187,52 +1175,44 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="33">
-        <v>0</v>
-      </c>
-      <c r="D14" s="14"/>
+        <v>11</v>
+      </c>
+      <c r="C14" s="29">
+        <v>7.4534161490683237E-3</v>
+      </c>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="11">
-        <f>215000*0.9</f>
-        <v>193500</v>
-      </c>
-      <c r="D15" s="16">
-        <v>310000</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C15" s="29">
+        <v>2.4844720496894411E-4</v>
+      </c>
+      <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="21">
-        <v>11000</v>
+        <v>0</v>
+      </c>
+      <c r="C16" s="11">
+        <f>215000*0.9</f>
+        <v>193500</v>
       </c>
       <c r="D16" s="16">
-        <v>11000</v>
+        <v>310000</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1240,13 +1220,13 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="23">
-        <v>18452.755905511811</v>
+        <v>10</v>
+      </c>
+      <c r="C17" s="21">
+        <v>11000</v>
       </c>
       <c r="D17" s="16">
-        <v>70000</v>
+        <v>11000</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -1260,10 +1240,10 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="23">
-        <v>1520.1354979368996</v>
+        <v>6</v>
+      </c>
+      <c r="C18" s="30">
+        <v>12877.712094925999</v>
       </c>
       <c r="D18" s="16">
         <v>70000</v>
@@ -1272,7 +1252,7 @@
         <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1280,164 +1260,178 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="23">
-        <v>0</v>
-      </c>
-      <c r="D19" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="C19" s="30">
+        <v>2121.0349332819292</v>
+      </c>
+      <c r="D19" s="16">
+        <v>70000</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="13">
-        <v>3</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>41</v>
-      </c>
+      <c r="C20" s="30">
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="D20" s="16"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="13">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" t="s">
-        <v>41</v>
-      </c>
+      <c r="C21" s="30">
+        <v>395.10377176636888</v>
+      </c>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="13">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="13">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="13">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="13">
-        <v>2.5</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="13">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0.5</v>
+      <c r="A30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B31" s="6">
         <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="7">
-        <f>SUM(B30:B31)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>24</v>
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="7">
+        <f>SUM(B31:B32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1465,25 +1459,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="29" t="str">
+      <c r="B2" s="26" t="str">
         <f>portfolio_input!B3</f>
         <v>Current Projects Portfolio</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>92</v>
+      <c r="A3" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="B3" t="str">
         <f>portfolio_input!G3</f>
@@ -1491,18 +1485,18 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="30">
+      <c r="A4" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="27">
         <v>45322</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="29" t="str">
+      <c r="A5" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="26" t="str">
         <f>portfolio_input!D3</f>
         <v>This portfolio describes The Current Projects portfolio reflects clean energy development projects that are being planned for or under way in the SJV. THIS PORTFOLIO ONLY USES BIOGAS TO PRODUCE BIOMETHANE FOR THE GAS GRID WHILE WE UPDATE THE MODEL.</v>
       </c>
@@ -1514,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225537EC-F8DB-7B4E-B90C-2D6AA935C6A7}">
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1529,19 +1523,19 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>64</v>
       </c>
       <c r="F1">
         <v>2025</v>
@@ -1612,55 +1606,55 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="E2" t="s">
-        <v>67</v>
-      </c>
       <c r="F2">
-        <f t="shared" ref="F2:F13" si="0">$P2/11</f>
+        <f>$P2/11</f>
         <v>1209.090909090909</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G13" si="1">$P2/11+F2</f>
+        <f>$P2/11+F2</f>
         <v>2418.181818181818</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:O2" si="2">$P2/11+G2</f>
+        <f t="shared" ref="H2:O2" si="0">$P2/11+G2</f>
         <v>3627.272727272727</v>
       </c>
       <c r="I2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4836.363636363636</v>
       </c>
       <c r="J2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>6045.454545454545</v>
       </c>
       <c r="K2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7254.545454545454</v>
       </c>
       <c r="L2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>8463.636363636364</v>
       </c>
       <c r="M2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>9672.7272727272721</v>
       </c>
       <c r="N2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10881.81818181818</v>
       </c>
       <c r="O2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>12090.909090909088</v>
       </c>
       <c r="P2">
@@ -1668,43 +1662,43 @@
         <v>13300</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q13" si="3">$P2</f>
+        <f>$P2</f>
         <v>13300</v>
       </c>
       <c r="R2">
-        <f t="shared" ref="R2:Z2" si="4">$P2</f>
+        <f t="shared" ref="R2:Z2" si="1">$P2</f>
         <v>13300</v>
       </c>
       <c r="S2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>13300</v>
       </c>
       <c r="T2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>13300</v>
       </c>
       <c r="U2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>13300</v>
       </c>
       <c r="V2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>13300</v>
       </c>
       <c r="W2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>13300</v>
       </c>
       <c r="X2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>13300</v>
       </c>
       <c r="Y2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>13300</v>
       </c>
       <c r="Z2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>13300</v>
       </c>
     </row>
@@ -1713,55 +1707,55 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>66</v>
       </c>
-      <c r="E3" t="s">
-        <v>67</v>
-      </c>
       <c r="F3">
-        <f t="shared" si="0"/>
+        <f>$P3/11</f>
         <v>24.545454545454547</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
+        <f>$P3/11+F3</f>
         <v>49.090909090909093</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:O13" si="5">$P3/11+G3</f>
+        <f>$P3/11+G3</f>
         <v>73.63636363636364</v>
       </c>
       <c r="I3">
-        <f t="shared" si="5"/>
+        <f>$P3/11+H3</f>
         <v>98.181818181818187</v>
       </c>
       <c r="J3">
-        <f t="shared" si="5"/>
+        <f>$P3/11+I3</f>
         <v>122.72727272727273</v>
       </c>
       <c r="K3">
-        <f t="shared" si="5"/>
+        <f>$P3/11+J3</f>
         <v>147.27272727272728</v>
       </c>
       <c r="L3">
-        <f t="shared" si="5"/>
+        <f>$P3/11+K3</f>
         <v>171.81818181818181</v>
       </c>
       <c r="M3">
-        <f t="shared" si="5"/>
+        <f>$P3/11+L3</f>
         <v>196.36363636363637</v>
       </c>
       <c r="N3">
-        <f t="shared" si="5"/>
+        <f>$P3/11+M3</f>
         <v>220.90909090909093</v>
       </c>
       <c r="O3">
-        <f t="shared" si="5"/>
+        <f>$P3/11+N3</f>
         <v>245.4545454545455</v>
       </c>
       <c r="P3">
@@ -1769,43 +1763,43 @@
         <v>270</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="3"/>
+        <f>$P3</f>
         <v>270</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:Z13" si="6">$P3</f>
+        <f>$P3</f>
         <v>270</v>
       </c>
       <c r="S3">
-        <f t="shared" si="6"/>
+        <f>$P3</f>
         <v>270</v>
       </c>
       <c r="T3">
-        <f t="shared" si="6"/>
+        <f>$P3</f>
         <v>270</v>
       </c>
       <c r="U3">
-        <f t="shared" si="6"/>
+        <f>$P3</f>
         <v>270</v>
       </c>
       <c r="V3">
-        <f t="shared" si="6"/>
+        <f>$P3</f>
         <v>270</v>
       </c>
       <c r="W3">
-        <f t="shared" si="6"/>
+        <f>$P3</f>
         <v>270</v>
       </c>
       <c r="X3">
-        <f t="shared" si="6"/>
+        <f>$P3</f>
         <v>270</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="6"/>
+        <f>$P3</f>
         <v>270</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="6"/>
+        <f>$P3</f>
         <v>270</v>
       </c>
     </row>
@@ -1814,55 +1808,55 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
         <v>66</v>
       </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f>$P4/11</f>
         <v>672.72727272727275</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f>$P4/11+F4</f>
         <v>1345.4545454545455</v>
       </c>
       <c r="H4">
-        <f t="shared" si="5"/>
+        <f>$P4/11+G4</f>
         <v>2018.1818181818182</v>
       </c>
       <c r="I4">
-        <f t="shared" si="5"/>
+        <f>$P4/11+H4</f>
         <v>2690.909090909091</v>
       </c>
       <c r="J4">
-        <f t="shared" si="5"/>
+        <f>$P4/11+I4</f>
         <v>3363.636363636364</v>
       </c>
       <c r="K4">
-        <f t="shared" si="5"/>
+        <f>$P4/11+J4</f>
         <v>4036.3636363636369</v>
       </c>
       <c r="L4">
-        <f t="shared" si="5"/>
+        <f>$P4/11+K4</f>
         <v>4709.0909090909099</v>
       </c>
       <c r="M4">
-        <f t="shared" si="5"/>
+        <f>$P4/11+L4</f>
         <v>5381.8181818181829</v>
       </c>
       <c r="N4">
-        <f t="shared" si="5"/>
+        <f>$P4/11+M4</f>
         <v>6054.5454545454559</v>
       </c>
       <c r="O4">
-        <f t="shared" si="5"/>
+        <f>$P4/11+N4</f>
         <v>6727.2727272727288</v>
       </c>
       <c r="P4">
@@ -1870,43 +1864,43 @@
         <v>7400</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="3"/>
+        <f>$P4</f>
         <v>7400</v>
       </c>
       <c r="R4">
-        <f t="shared" si="6"/>
+        <f>$P4</f>
         <v>7400</v>
       </c>
       <c r="S4">
-        <f t="shared" si="6"/>
+        <f>$P4</f>
         <v>7400</v>
       </c>
       <c r="T4">
-        <f t="shared" si="6"/>
+        <f>$P4</f>
         <v>7400</v>
       </c>
       <c r="U4">
-        <f t="shared" si="6"/>
+        <f>$P4</f>
         <v>7400</v>
       </c>
       <c r="V4">
-        <f t="shared" si="6"/>
+        <f>$P4</f>
         <v>7400</v>
       </c>
       <c r="W4">
-        <f t="shared" si="6"/>
+        <f>$P4</f>
         <v>7400</v>
       </c>
       <c r="X4">
-        <f t="shared" si="6"/>
+        <f>$P4</f>
         <v>7400</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="6"/>
+        <f>$P4</f>
         <v>7400</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="6"/>
+        <f>$P4</f>
         <v>7400</v>
       </c>
     </row>
@@ -1915,55 +1909,55 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
         <v>66</v>
       </c>
-      <c r="E5" t="s">
-        <v>67</v>
-      </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f>$P5/11</f>
         <v>90.909090909090907</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f>$P5/11+F5</f>
         <v>181.81818181818181</v>
       </c>
       <c r="H5">
-        <f t="shared" si="5"/>
+        <f>$P5/11+G5</f>
         <v>272.72727272727275</v>
       </c>
       <c r="I5">
-        <f t="shared" si="5"/>
+        <f>$P5/11+H5</f>
         <v>363.63636363636363</v>
       </c>
       <c r="J5">
-        <f t="shared" si="5"/>
+        <f>$P5/11+I5</f>
         <v>454.5454545454545</v>
       </c>
       <c r="K5">
-        <f t="shared" si="5"/>
+        <f>$P5/11+J5</f>
         <v>545.45454545454538</v>
       </c>
       <c r="L5">
-        <f t="shared" si="5"/>
+        <f>$P5/11+K5</f>
         <v>636.36363636363626</v>
       </c>
       <c r="M5">
-        <f t="shared" si="5"/>
+        <f>$P5/11+L5</f>
         <v>727.27272727272714</v>
       </c>
       <c r="N5">
-        <f t="shared" si="5"/>
+        <f>$P5/11+M5</f>
         <v>818.18181818181802</v>
       </c>
       <c r="O5">
-        <f t="shared" si="5"/>
+        <f>$P5/11+N5</f>
         <v>909.09090909090889</v>
       </c>
       <c r="P5">
@@ -1971,456 +1965,456 @@
         <v>1000</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="3"/>
+        <f>$P5</f>
         <v>1000</v>
       </c>
       <c r="R5">
-        <f t="shared" si="6"/>
+        <f>$P5</f>
         <v>1000</v>
       </c>
       <c r="S5">
-        <f t="shared" si="6"/>
+        <f>$P5</f>
         <v>1000</v>
       </c>
       <c r="T5">
-        <f t="shared" si="6"/>
+        <f>$P5</f>
         <v>1000</v>
       </c>
       <c r="U5">
-        <f t="shared" si="6"/>
+        <f>$P5</f>
         <v>1000</v>
       </c>
       <c r="V5">
-        <f t="shared" si="6"/>
+        <f>$P5</f>
         <v>1000</v>
       </c>
       <c r="W5">
-        <f t="shared" si="6"/>
+        <f>$P5</f>
         <v>1000</v>
       </c>
       <c r="X5">
-        <f t="shared" si="6"/>
+        <f>$P5</f>
         <v>1000</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="6"/>
+        <f>$P5</f>
         <v>1000</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="6"/>
+        <f>$P5</f>
         <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" t="s">
-        <v>67</v>
-      </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>1.5610651974288337</v>
+        <f>$P6/11</f>
+        <v>0.9599096555618295</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
-        <v>3.1221303948576673</v>
+        <f>$P6/11+F6</f>
+        <v>1.919819311123659</v>
       </c>
       <c r="H6">
-        <f t="shared" si="5"/>
-        <v>4.6831955922865012</v>
+        <f>$P6/11+G6</f>
+        <v>2.8797289666854886</v>
       </c>
       <c r="I6">
-        <f t="shared" si="5"/>
-        <v>6.2442607897153346</v>
+        <f>$P6/11+H6</f>
+        <v>3.839638622247318</v>
       </c>
       <c r="J6">
-        <f t="shared" si="5"/>
-        <v>7.805325987144168</v>
+        <f>$P6/11+I6</f>
+        <v>4.7995482778091478</v>
       </c>
       <c r="K6">
-        <f t="shared" si="5"/>
-        <v>9.3663911845730023</v>
+        <f>$P6/11+J6</f>
+        <v>5.7594579333709772</v>
       </c>
       <c r="L6">
-        <f t="shared" si="5"/>
-        <v>10.927456382001836</v>
+        <f>$P6/11+K6</f>
+        <v>6.7193675889328066</v>
       </c>
       <c r="M6">
-        <f t="shared" si="5"/>
-        <v>12.488521579430669</v>
+        <f>$P6/11+L6</f>
+        <v>7.679277244494636</v>
       </c>
       <c r="N6">
-        <f t="shared" si="5"/>
-        <v>14.049586776859503</v>
+        <f>$P6/11+M6</f>
+        <v>8.6391869000564654</v>
       </c>
       <c r="O6">
-        <f t="shared" si="5"/>
-        <v>15.610651974288336</v>
+        <f>$P6/11+N6</f>
+        <v>9.5990965556182957</v>
       </c>
       <c r="P6">
         <f>portfolio_input!C12*1000</f>
-        <v>17.171717171717169</v>
+        <v>10.559006211180124</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="3"/>
-        <v>17.171717171717169</v>
+        <f>$P6</f>
+        <v>10.559006211180124</v>
       </c>
       <c r="R6">
-        <f t="shared" si="6"/>
-        <v>17.171717171717169</v>
+        <f>$P6</f>
+        <v>10.559006211180124</v>
       </c>
       <c r="S6">
-        <f t="shared" si="6"/>
-        <v>17.171717171717169</v>
+        <f>$P6</f>
+        <v>10.559006211180124</v>
       </c>
       <c r="T6">
-        <f t="shared" si="6"/>
-        <v>17.171717171717169</v>
+        <f>$P6</f>
+        <v>10.559006211180124</v>
       </c>
       <c r="U6">
-        <f t="shared" si="6"/>
-        <v>17.171717171717169</v>
+        <f>$P6</f>
+        <v>10.559006211180124</v>
       </c>
       <c r="V6">
-        <f t="shared" si="6"/>
-        <v>17.171717171717169</v>
+        <f>$P6</f>
+        <v>10.559006211180124</v>
       </c>
       <c r="W6">
-        <f t="shared" si="6"/>
-        <v>17.171717171717169</v>
+        <f>$P6</f>
+        <v>10.559006211180124</v>
       </c>
       <c r="X6">
-        <f t="shared" si="6"/>
-        <v>17.171717171717169</v>
+        <f>$P6</f>
+        <v>10.559006211180124</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="6"/>
-        <v>17.171717171717169</v>
+        <f>$P6</f>
+        <v>10.559006211180124</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="6"/>
-        <v>17.171717171717169</v>
+        <f>$P6</f>
+        <v>10.559006211180124</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
         <v>66</v>
       </c>
-      <c r="E7" t="s">
-        <v>67</v>
-      </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0.25711662075298441</v>
+        <f>$P7/11</f>
+        <v>0.15810276679841898</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
-        <v>0.51423324150596883</v>
+        <f>$P7/11+F7</f>
+        <v>0.31620553359683795</v>
       </c>
       <c r="H7">
-        <f t="shared" si="5"/>
-        <v>0.77134986225895319</v>
+        <f>$P7/11+G7</f>
+        <v>0.47430830039525695</v>
       </c>
       <c r="I7">
-        <f t="shared" si="5"/>
-        <v>1.0284664830119377</v>
+        <f>$P7/11+H7</f>
+        <v>0.6324110671936759</v>
       </c>
       <c r="J7">
-        <f t="shared" si="5"/>
-        <v>1.2855831037649221</v>
+        <f>$P7/11+I7</f>
+        <v>0.79051383399209485</v>
       </c>
       <c r="K7">
-        <f t="shared" si="5"/>
-        <v>1.5426997245179066</v>
+        <f>$P7/11+J7</f>
+        <v>0.9486166007905138</v>
       </c>
       <c r="L7">
-        <f t="shared" si="5"/>
-        <v>1.7998163452708911</v>
+        <f>$P7/11+K7</f>
+        <v>1.1067193675889329</v>
       </c>
       <c r="M7">
-        <f t="shared" si="5"/>
-        <v>2.0569329660238753</v>
+        <f>$P7/11+L7</f>
+        <v>1.2648221343873518</v>
       </c>
       <c r="N7">
-        <f t="shared" si="5"/>
-        <v>2.3140495867768598</v>
+        <f>$P7/11+M7</f>
+        <v>1.4229249011857708</v>
       </c>
       <c r="O7">
-        <f t="shared" si="5"/>
-        <v>2.5711662075298443</v>
+        <f>$P7/11+N7</f>
+        <v>1.5810276679841897</v>
       </c>
       <c r="P7">
         <f>portfolio_input!C13*1000</f>
-        <v>2.8282828282828287</v>
+        <v>1.7391304347826089</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="3"/>
-        <v>2.8282828282828287</v>
+        <f>$P7</f>
+        <v>1.7391304347826089</v>
       </c>
       <c r="R7">
-        <f t="shared" si="6"/>
-        <v>2.8282828282828287</v>
+        <f>$P7</f>
+        <v>1.7391304347826089</v>
       </c>
       <c r="S7">
-        <f t="shared" si="6"/>
-        <v>2.8282828282828287</v>
+        <f>$P7</f>
+        <v>1.7391304347826089</v>
       </c>
       <c r="T7">
-        <f t="shared" si="6"/>
-        <v>2.8282828282828287</v>
+        <f>$P7</f>
+        <v>1.7391304347826089</v>
       </c>
       <c r="U7">
-        <f t="shared" si="6"/>
-        <v>2.8282828282828287</v>
+        <f>$P7</f>
+        <v>1.7391304347826089</v>
       </c>
       <c r="V7">
-        <f t="shared" si="6"/>
-        <v>2.8282828282828287</v>
+        <f>$P7</f>
+        <v>1.7391304347826089</v>
       </c>
       <c r="W7">
-        <f t="shared" si="6"/>
-        <v>2.8282828282828287</v>
+        <f>$P7</f>
+        <v>1.7391304347826089</v>
       </c>
       <c r="X7">
-        <f t="shared" si="6"/>
-        <v>2.8282828282828287</v>
+        <f>$P7</f>
+        <v>1.7391304347826089</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="6"/>
-        <v>2.8282828282828287</v>
+        <f>$P7</f>
+        <v>1.7391304347826089</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="6"/>
-        <v>2.8282828282828287</v>
+        <f>$P7</f>
+        <v>1.7391304347826089</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" t="s">
         <v>66</v>
       </c>
-      <c r="E8" t="s">
-        <v>67</v>
-      </c>
       <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="F8:F9" si="2">$P8/11</f>
+        <v>0.67758328627893849</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="G8:O9" si="3">$P8/11+F8</f>
+        <v>1.355166572557877</v>
       </c>
       <c r="H8">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2.0327498588368154</v>
       </c>
       <c r="I8">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>2.710333145115754</v>
       </c>
       <c r="J8">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3.3879164313946926</v>
       </c>
       <c r="K8">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>4.0654997176736307</v>
       </c>
       <c r="L8">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>4.7430830039525693</v>
       </c>
       <c r="M8">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>5.4206662902315079</v>
       </c>
       <c r="N8">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>6.0982495765104465</v>
       </c>
       <c r="O8">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>6.7758328627893851</v>
       </c>
       <c r="P8">
         <f>portfolio_input!C14*1000</f>
-        <v>0</v>
+        <v>7.4534161490683237</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="Q8:Z9" si="4">$P8</f>
+        <v>7.4534161490683237</v>
       </c>
       <c r="R8">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>7.4534161490683237</v>
       </c>
       <c r="S8">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>7.4534161490683237</v>
       </c>
       <c r="T8">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>7.4534161490683237</v>
       </c>
       <c r="U8">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>7.4534161490683237</v>
       </c>
       <c r="V8">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>7.4534161490683237</v>
       </c>
       <c r="W8">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>7.4534161490683237</v>
       </c>
       <c r="X8">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>7.4534161490683237</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>7.4534161490683237</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>7.4534161490683237</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
-        <v>17590.909090909092</v>
+        <f t="shared" si="2"/>
+        <v>2.258610954263128E-2</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>35181.818181818184</v>
+        <f t="shared" si="3"/>
+        <v>4.517221908526256E-2</v>
       </c>
       <c r="H9">
-        <f t="shared" si="5"/>
-        <v>52772.727272727279</v>
+        <f t="shared" si="3"/>
+        <v>6.7758328627893841E-2</v>
       </c>
       <c r="I9">
-        <f t="shared" si="5"/>
-        <v>70363.636363636368</v>
+        <f t="shared" si="3"/>
+        <v>9.0344438170525121E-2</v>
       </c>
       <c r="J9">
-        <f t="shared" si="5"/>
-        <v>87954.545454545456</v>
+        <f t="shared" si="3"/>
+        <v>0.1129305477131564</v>
       </c>
       <c r="K9">
-        <f t="shared" si="5"/>
-        <v>105545.45454545454</v>
+        <f t="shared" si="3"/>
+        <v>0.13551665725578768</v>
       </c>
       <c r="L9">
-        <f t="shared" si="5"/>
-        <v>123136.36363636363</v>
+        <f t="shared" si="3"/>
+        <v>0.15810276679841895</v>
       </c>
       <c r="M9">
-        <f t="shared" si="5"/>
-        <v>140727.27272727274</v>
+        <f t="shared" si="3"/>
+        <v>0.18068887634105024</v>
       </c>
       <c r="N9">
-        <f t="shared" si="5"/>
-        <v>158318.18181818182</v>
+        <f t="shared" si="3"/>
+        <v>0.20327498588368154</v>
       </c>
       <c r="O9">
-        <f t="shared" si="5"/>
-        <v>175909.09090909091</v>
-      </c>
-      <c r="P9" s="25">
-        <f>215000*0.9</f>
-        <v>193500</v>
+        <f t="shared" si="3"/>
+        <v>0.22586109542631283</v>
+      </c>
+      <c r="P9">
+        <f>portfolio_input!C15*1000</f>
+        <v>0.2484472049689441</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="3"/>
-        <v>193500</v>
+        <f t="shared" si="4"/>
+        <v>0.2484472049689441</v>
       </c>
       <c r="R9">
-        <f t="shared" si="6"/>
-        <v>193500</v>
+        <f t="shared" si="4"/>
+        <v>0.2484472049689441</v>
       </c>
       <c r="S9">
-        <f t="shared" si="6"/>
-        <v>193500</v>
+        <f t="shared" si="4"/>
+        <v>0.2484472049689441</v>
       </c>
       <c r="T9">
-        <f t="shared" si="6"/>
-        <v>193500</v>
+        <f t="shared" si="4"/>
+        <v>0.2484472049689441</v>
       </c>
       <c r="U9">
-        <f t="shared" si="6"/>
-        <v>193500</v>
+        <f t="shared" si="4"/>
+        <v>0.2484472049689441</v>
       </c>
       <c r="V9">
-        <f t="shared" si="6"/>
-        <v>193500</v>
+        <f t="shared" si="4"/>
+        <v>0.2484472049689441</v>
       </c>
       <c r="W9">
-        <f t="shared" si="6"/>
-        <v>193500</v>
+        <f t="shared" si="4"/>
+        <v>0.2484472049689441</v>
       </c>
       <c r="X9">
-        <f t="shared" si="6"/>
-        <v>193500</v>
+        <f t="shared" si="4"/>
+        <v>0.2484472049689441</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="6"/>
-        <v>193500</v>
+        <f t="shared" si="4"/>
+        <v>0.2484472049689441</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="6"/>
-        <v>193500</v>
+        <f t="shared" si="4"/>
+        <v>0.2484472049689441</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2429,98 +2423,99 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <f>$P10/11</f>
+        <v>17590.909090909092</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
-        <v>2000</v>
+        <f>$P10/11+F10</f>
+        <v>35181.818181818184</v>
       </c>
       <c r="H10">
-        <f t="shared" si="5"/>
-        <v>3000</v>
+        <f>$P10/11+G10</f>
+        <v>52772.727272727279</v>
       </c>
       <c r="I10">
-        <f t="shared" si="5"/>
-        <v>4000</v>
+        <f>$P10/11+H10</f>
+        <v>70363.636363636368</v>
       </c>
       <c r="J10">
-        <f t="shared" si="5"/>
-        <v>5000</v>
+        <f>$P10/11+I10</f>
+        <v>87954.545454545456</v>
       </c>
       <c r="K10">
-        <f t="shared" si="5"/>
-        <v>6000</v>
+        <f>$P10/11+J10</f>
+        <v>105545.45454545454</v>
       </c>
       <c r="L10">
-        <f t="shared" si="5"/>
-        <v>7000</v>
+        <f>$P10/11+K10</f>
+        <v>123136.36363636363</v>
       </c>
       <c r="M10">
-        <f t="shared" si="5"/>
-        <v>8000</v>
+        <f>$P10/11+L10</f>
+        <v>140727.27272727274</v>
       </c>
       <c r="N10">
-        <f t="shared" si="5"/>
-        <v>9000</v>
+        <f>$P10/11+M10</f>
+        <v>158318.18181818182</v>
       </c>
       <c r="O10">
-        <f t="shared" si="5"/>
-        <v>10000</v>
-      </c>
-      <c r="P10" s="26">
-        <v>11000</v>
+        <f>$P10/11+N10</f>
+        <v>175909.09090909091</v>
+      </c>
+      <c r="P10" s="24">
+        <f>portfolio_input!C16</f>
+        <v>193500</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="3"/>
-        <v>11000</v>
+        <f>$P10</f>
+        <v>193500</v>
       </c>
       <c r="R10">
-        <f t="shared" si="6"/>
-        <v>11000</v>
+        <f>$P10</f>
+        <v>193500</v>
       </c>
       <c r="S10">
-        <f t="shared" si="6"/>
-        <v>11000</v>
+        <f>$P10</f>
+        <v>193500</v>
       </c>
       <c r="T10">
-        <f t="shared" si="6"/>
-        <v>11000</v>
+        <f>$P10</f>
+        <v>193500</v>
       </c>
       <c r="U10">
-        <f t="shared" si="6"/>
-        <v>11000</v>
+        <f>$P10</f>
+        <v>193500</v>
       </c>
       <c r="V10">
-        <f t="shared" si="6"/>
-        <v>11000</v>
+        <f>$P10</f>
+        <v>193500</v>
       </c>
       <c r="W10">
-        <f t="shared" si="6"/>
-        <v>11000</v>
+        <f>$P10</f>
+        <v>193500</v>
       </c>
       <c r="X10">
-        <f t="shared" si="6"/>
-        <v>11000</v>
+        <f>$P10</f>
+        <v>193500</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="6"/>
-        <v>11000</v>
+        <f>$P10</f>
+        <v>193500</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="6"/>
-        <v>11000</v>
+        <f>$P10</f>
+        <v>193500</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2529,98 +2524,99 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>975</v>
+        <f>$P11/11</f>
+        <v>1000</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
-        <v>1950</v>
+        <f>$P11/11+F11</f>
+        <v>2000</v>
       </c>
       <c r="H11">
-        <f t="shared" si="5"/>
-        <v>2925</v>
+        <f>$P11/11+G11</f>
+        <v>3000</v>
       </c>
       <c r="I11">
-        <f t="shared" si="5"/>
-        <v>3900</v>
+        <f>$P11/11+H11</f>
+        <v>4000</v>
       </c>
       <c r="J11">
-        <f t="shared" si="5"/>
-        <v>4875</v>
+        <f>$P11/11+I11</f>
+        <v>5000</v>
       </c>
       <c r="K11">
-        <f t="shared" si="5"/>
-        <v>5850</v>
+        <f>$P11/11+J11</f>
+        <v>6000</v>
       </c>
       <c r="L11">
-        <f t="shared" si="5"/>
-        <v>6825</v>
+        <f>$P11/11+K11</f>
+        <v>7000</v>
       </c>
       <c r="M11">
-        <f t="shared" si="5"/>
-        <v>7800</v>
+        <f>$P11/11+L11</f>
+        <v>8000</v>
       </c>
       <c r="N11">
-        <f t="shared" si="5"/>
-        <v>8775</v>
+        <f>$P11/11+M11</f>
+        <v>9000</v>
       </c>
       <c r="O11">
-        <f t="shared" si="5"/>
-        <v>9750</v>
-      </c>
-      <c r="P11" s="28">
-        <v>10725</v>
+        <f>$P11/11+N11</f>
+        <v>10000</v>
+      </c>
+      <c r="P11" s="24">
+        <f>portfolio_input!C17</f>
+        <v>11000</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="3"/>
-        <v>10725</v>
+        <f>$P11</f>
+        <v>11000</v>
       </c>
       <c r="R11">
-        <f t="shared" si="6"/>
-        <v>10725</v>
+        <f>$P11</f>
+        <v>11000</v>
       </c>
       <c r="S11">
-        <f t="shared" si="6"/>
-        <v>10725</v>
+        <f>$P11</f>
+        <v>11000</v>
       </c>
       <c r="T11">
-        <f t="shared" si="6"/>
-        <v>10725</v>
+        <f>$P11</f>
+        <v>11000</v>
       </c>
       <c r="U11">
-        <f t="shared" si="6"/>
-        <v>10725</v>
+        <f>$P11</f>
+        <v>11000</v>
       </c>
       <c r="V11">
-        <f t="shared" si="6"/>
-        <v>10725</v>
+        <f>$P11</f>
+        <v>11000</v>
       </c>
       <c r="W11">
-        <f t="shared" si="6"/>
-        <v>10725</v>
+        <f>$P11</f>
+        <v>11000</v>
       </c>
       <c r="X11">
-        <f t="shared" si="6"/>
-        <v>10725</v>
+        <f>$P11</f>
+        <v>11000</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="6"/>
-        <v>10725</v>
+        <f>$P11</f>
+        <v>11000</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="6"/>
-        <v>10725</v>
+        <f>$P11</f>
+        <v>11000</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2629,98 +2625,99 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
-        <v>161</v>
+        <f>$P12/11</f>
+        <v>1170.7010995387272</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
-        <v>322</v>
+        <f>$P12/11+F12</f>
+        <v>2341.4021990774545</v>
       </c>
       <c r="H12">
-        <f t="shared" si="5"/>
-        <v>483</v>
+        <f>$P12/11+G12</f>
+        <v>3512.1032986161817</v>
       </c>
       <c r="I12">
-        <f t="shared" si="5"/>
-        <v>644</v>
+        <f>$P12/11+H12</f>
+        <v>4682.804398154909</v>
       </c>
       <c r="J12">
-        <f t="shared" si="5"/>
-        <v>805</v>
+        <f>$P12/11+I12</f>
+        <v>5853.5054976936362</v>
       </c>
       <c r="K12">
-        <f t="shared" si="5"/>
-        <v>966</v>
+        <f>$P12/11+J12</f>
+        <v>7024.2065972323635</v>
       </c>
       <c r="L12">
-        <f t="shared" si="5"/>
-        <v>1127</v>
+        <f>$P12/11+K12</f>
+        <v>8194.9076967710898</v>
       </c>
       <c r="M12">
-        <f t="shared" si="5"/>
-        <v>1288</v>
+        <f>$P12/11+L12</f>
+        <v>9365.608796309818</v>
       </c>
       <c r="N12">
-        <f t="shared" si="5"/>
-        <v>1449</v>
+        <f>$P12/11+M12</f>
+        <v>10536.309895848546</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
-        <v>1610</v>
-      </c>
-      <c r="P12" s="28">
-        <v>1771</v>
+        <f>$P12/11+N12</f>
+        <v>11707.010995387274</v>
+      </c>
+      <c r="P12" s="24">
+        <f>portfolio_input!C18</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="3"/>
-        <v>1771</v>
+        <f>$P12</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="R12">
-        <f t="shared" si="6"/>
-        <v>1771</v>
+        <f>$P12</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="S12">
-        <f t="shared" si="6"/>
-        <v>1771</v>
+        <f>$P12</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="T12">
-        <f t="shared" si="6"/>
-        <v>1771</v>
+        <f>$P12</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="U12">
-        <f t="shared" si="6"/>
-        <v>1771</v>
+        <f>$P12</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="V12">
-        <f t="shared" si="6"/>
-        <v>1771</v>
+        <f>$P12</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="W12">
-        <f t="shared" si="6"/>
-        <v>1771</v>
+        <f>$P12</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="X12">
-        <f t="shared" si="6"/>
-        <v>1771</v>
+        <f>$P12</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="6"/>
-        <v>1771</v>
+        <f>$P12</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="6"/>
-        <v>1771</v>
+        <f>$P12</f>
+        <v>12877.712094925999</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -2729,91 +2726,91 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>$P13/11</f>
+        <v>192.82135757108446</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>$P13/11+F13</f>
+        <v>385.64271514216892</v>
       </c>
       <c r="H13">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" ref="H13:O13" si="5">$P13/11+G13</f>
+        <v>578.46407271325336</v>
       </c>
       <c r="I13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>771.28543028433785</v>
       </c>
       <c r="J13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>964.10678785542234</v>
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1156.9281454265067</v>
       </c>
       <c r="L13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1349.7495029975912</v>
       </c>
       <c r="M13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1542.5708605686757</v>
       </c>
       <c r="N13">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1735.3922181397602</v>
       </c>
       <c r="O13">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="28">
+        <v>1928.2135757108447</v>
+      </c>
+      <c r="P13" s="24">
         <f>portfolio_input!C19</f>
-        <v>0</v>
+        <v>2121.0349332819292</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>$P13</f>
+        <v>2121.0349332819292</v>
       </c>
       <c r="R13">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" ref="R13:Z13" si="6">$P13</f>
+        <v>2121.0349332819292</v>
       </c>
       <c r="S13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2121.0349332819292</v>
       </c>
       <c r="T13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2121.0349332819292</v>
       </c>
       <c r="U13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2121.0349332819292</v>
       </c>
       <c r="V13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2121.0349332819292</v>
       </c>
       <c r="W13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2121.0349332819292</v>
       </c>
       <c r="X13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2121.0349332819292</v>
       </c>
       <c r="Y13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2121.0349332819292</v>
       </c>
       <c r="Z13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2121.0349332819292</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
@@ -2821,85 +2818,287 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
-      </c>
-      <c r="P14" s="27"/>
+        <v>72</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F15" si="7">$P14/11</f>
+        <v>555.10447272960926</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:O15" si="8">$P14/11+F14</f>
+        <v>1110.2089454592185</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="8"/>
+        <v>1665.3134181888277</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="8"/>
+        <v>2220.417890918437</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="8"/>
+        <v>2775.5223636480464</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="8"/>
+        <v>3330.6268363776558</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="8"/>
+        <v>3885.7313091072651</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="8"/>
+        <v>4440.835781836874</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="8"/>
+        <v>4995.9402545664834</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="8"/>
+        <v>5551.0447272960928</v>
+      </c>
+      <c r="P14" s="24">
+        <f>portfolio_input!C20</f>
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" ref="Q14:Z15" si="9">$P14</f>
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="9"/>
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="9"/>
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="9"/>
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="9"/>
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="9"/>
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="9"/>
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="9"/>
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="9"/>
+        <v>6106.1492000257012</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="9"/>
+        <v>6106.1492000257012</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="7"/>
+        <v>35.918524706033537</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="8"/>
+        <v>71.837049412067074</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="8"/>
+        <v>107.75557411810061</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="8"/>
+        <v>143.67409882413415</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="8"/>
+        <v>179.59262353016769</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="8"/>
+        <v>215.51114823620122</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="8"/>
+        <v>251.42967294223476</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="8"/>
+        <v>287.3481976482683</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="8"/>
+        <v>323.26672235430181</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="8"/>
+        <v>359.18524706033531</v>
+      </c>
+      <c r="P15" s="24">
+        <f>portfolio_input!C21</f>
+        <v>395.10377176636888</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="9"/>
+        <v>395.10377176636888</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="9"/>
+        <v>395.10377176636888</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="9"/>
+        <v>395.10377176636888</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="9"/>
+        <v>395.10377176636888</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="9"/>
+        <v>395.10377176636888</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="9"/>
+        <v>395.10377176636888</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="9"/>
+        <v>395.10377176636888</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="9"/>
+        <v>395.10377176636888</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="9"/>
+        <v>395.10377176636888</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="9"/>
+        <v>395.10377176636888</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="P16" s="25"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
-        <v>79</v>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2922,357 +3121,357 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="24" t="s">
+      <c r="A1" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="23">
+        <v>2025</v>
+      </c>
+      <c r="D1" s="23">
+        <v>2026</v>
+      </c>
+      <c r="E1" s="23">
+        <v>2027</v>
+      </c>
+      <c r="F1" s="23">
+        <v>2028</v>
+      </c>
+      <c r="G1" s="23">
+        <v>2029</v>
+      </c>
+      <c r="H1" s="23">
+        <v>2030</v>
+      </c>
+      <c r="I1" s="23">
+        <v>2031</v>
+      </c>
+      <c r="J1" s="23">
+        <v>2032</v>
+      </c>
+      <c r="K1" s="23">
+        <v>2033</v>
+      </c>
+      <c r="L1" s="23">
+        <v>2034</v>
+      </c>
+      <c r="M1" s="23">
+        <v>2035</v>
+      </c>
+      <c r="N1" s="23">
+        <v>2036</v>
+      </c>
+      <c r="O1" s="23">
+        <v>2037</v>
+      </c>
+      <c r="P1" s="23">
+        <v>2038</v>
+      </c>
+      <c r="Q1" s="23">
+        <v>2039</v>
+      </c>
+      <c r="R1" s="23">
+        <v>2040</v>
+      </c>
+      <c r="S1" s="23">
+        <v>2041</v>
+      </c>
+      <c r="T1" s="23">
+        <v>2042</v>
+      </c>
+      <c r="U1" s="23">
+        <v>2043</v>
+      </c>
+      <c r="V1" s="23">
+        <v>2044</v>
+      </c>
+      <c r="W1" s="23">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="24">
-        <v>2025</v>
-      </c>
-      <c r="D1" s="24">
-        <v>2026</v>
-      </c>
-      <c r="E1" s="24">
-        <v>2027</v>
-      </c>
-      <c r="F1" s="24">
-        <v>2028</v>
-      </c>
-      <c r="G1" s="24">
-        <v>2029</v>
-      </c>
-      <c r="H1" s="24">
-        <v>2030</v>
-      </c>
-      <c r="I1" s="24">
-        <v>2031</v>
-      </c>
-      <c r="J1" s="24">
-        <v>2032</v>
-      </c>
-      <c r="K1" s="24">
-        <v>2033</v>
-      </c>
-      <c r="L1" s="24">
-        <v>2034</v>
-      </c>
-      <c r="M1" s="24">
-        <v>2035</v>
-      </c>
-      <c r="N1" s="24">
-        <v>2036</v>
-      </c>
-      <c r="O1" s="24">
-        <v>2037</v>
-      </c>
-      <c r="P1" s="24">
-        <v>2038</v>
-      </c>
-      <c r="Q1" s="24">
-        <v>2039</v>
-      </c>
-      <c r="R1" s="24">
-        <v>2040</v>
-      </c>
-      <c r="S1" s="24">
-        <v>2041</v>
-      </c>
-      <c r="T1" s="24">
-        <v>2042</v>
-      </c>
-      <c r="U1" s="24">
-        <v>2043</v>
-      </c>
-      <c r="V1" s="24">
-        <v>2044</v>
-      </c>
-      <c r="W1" s="24">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="24" t="s">
+      <c r="C2" s="23">
+        <v>1</v>
+      </c>
+      <c r="D2" s="23">
+        <v>1</v>
+      </c>
+      <c r="E2" s="23">
+        <v>1</v>
+      </c>
+      <c r="F2" s="23">
+        <v>1</v>
+      </c>
+      <c r="G2" s="23">
+        <v>1</v>
+      </c>
+      <c r="H2" s="23">
+        <v>1</v>
+      </c>
+      <c r="I2" s="23">
+        <v>1</v>
+      </c>
+      <c r="J2" s="23">
+        <v>1</v>
+      </c>
+      <c r="K2" s="23">
+        <v>1</v>
+      </c>
+      <c r="L2" s="23">
+        <v>1</v>
+      </c>
+      <c r="M2" s="23">
+        <v>1</v>
+      </c>
+      <c r="N2" s="23">
+        <v>1</v>
+      </c>
+      <c r="O2" s="23">
+        <v>1</v>
+      </c>
+      <c r="P2" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="23">
+        <v>1</v>
+      </c>
+      <c r="R2" s="23">
+        <v>1</v>
+      </c>
+      <c r="S2" s="23">
+        <v>1</v>
+      </c>
+      <c r="T2" s="23">
+        <v>1</v>
+      </c>
+      <c r="U2" s="23">
+        <v>1</v>
+      </c>
+      <c r="V2" s="23">
+        <v>1</v>
+      </c>
+      <c r="W2" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="24">
-        <v>1</v>
-      </c>
-      <c r="D2" s="24">
-        <v>1</v>
-      </c>
-      <c r="E2" s="24">
-        <v>1</v>
-      </c>
-      <c r="F2" s="24">
-        <v>1</v>
-      </c>
-      <c r="G2" s="24">
-        <v>1</v>
-      </c>
-      <c r="H2" s="24">
-        <v>1</v>
-      </c>
-      <c r="I2" s="24">
-        <v>1</v>
-      </c>
-      <c r="J2" s="24">
-        <v>1</v>
-      </c>
-      <c r="K2" s="24">
-        <v>1</v>
-      </c>
-      <c r="L2" s="24">
-        <v>1</v>
-      </c>
-      <c r="M2" s="24">
-        <v>1</v>
-      </c>
-      <c r="N2" s="24">
-        <v>1</v>
-      </c>
-      <c r="O2" s="24">
-        <v>1</v>
-      </c>
-      <c r="P2" s="24">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="24">
-        <v>1</v>
-      </c>
-      <c r="R2" s="24">
-        <v>1</v>
-      </c>
-      <c r="S2" s="24">
-        <v>1</v>
-      </c>
-      <c r="T2" s="24">
-        <v>1</v>
-      </c>
-      <c r="U2" s="24">
-        <v>1</v>
-      </c>
-      <c r="V2" s="24">
-        <v>1</v>
-      </c>
-      <c r="W2" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="C3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="R3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="S3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="T3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="U3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="V3" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="W3" s="23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="F3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="J3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="L3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="M3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="N3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="O3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="P3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="Q3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="R3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="S3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="T3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="U3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="V3" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="W3" s="24">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="E4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="I4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="J4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="K4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="L4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="M4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="N4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="O4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="P4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="Q4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="R4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="S4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="T4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="U4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="V4" s="24">
-        <v>0.5</v>
-      </c>
-      <c r="W4" s="24">
+      <c r="C4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="O4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="R4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="S4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="T4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="U4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="V4" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="W4" s="23">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="24">
-        <v>1</v>
-      </c>
-      <c r="D5" s="24">
-        <v>1</v>
-      </c>
-      <c r="E5" s="24">
-        <v>1</v>
-      </c>
-      <c r="F5" s="24">
-        <v>1</v>
-      </c>
-      <c r="G5" s="24">
-        <v>1</v>
-      </c>
-      <c r="H5" s="24">
-        <v>1</v>
-      </c>
-      <c r="I5" s="24">
-        <v>1</v>
-      </c>
-      <c r="J5" s="24">
-        <v>1</v>
-      </c>
-      <c r="K5" s="24">
-        <v>1</v>
-      </c>
-      <c r="L5" s="24">
-        <v>1</v>
-      </c>
-      <c r="M5" s="24">
-        <v>1</v>
-      </c>
-      <c r="N5" s="24">
-        <v>1</v>
-      </c>
-      <c r="O5" s="24">
-        <v>1</v>
-      </c>
-      <c r="P5" s="24">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="24">
-        <v>1</v>
-      </c>
-      <c r="R5" s="24">
-        <v>1</v>
-      </c>
-      <c r="S5" s="24">
-        <v>1</v>
-      </c>
-      <c r="T5" s="24">
-        <v>1</v>
-      </c>
-      <c r="U5" s="24">
-        <v>1</v>
-      </c>
-      <c r="V5" s="24">
-        <v>1</v>
-      </c>
-      <c r="W5" s="24">
+      <c r="A5" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="23">
+        <v>1</v>
+      </c>
+      <c r="D5" s="23">
+        <v>1</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
+      <c r="F5" s="23">
+        <v>1</v>
+      </c>
+      <c r="G5" s="23">
+        <v>1</v>
+      </c>
+      <c r="H5" s="23">
+        <v>1</v>
+      </c>
+      <c r="I5" s="23">
+        <v>1</v>
+      </c>
+      <c r="J5" s="23">
+        <v>1</v>
+      </c>
+      <c r="K5" s="23">
+        <v>1</v>
+      </c>
+      <c r="L5" s="23">
+        <v>1</v>
+      </c>
+      <c r="M5" s="23">
+        <v>1</v>
+      </c>
+      <c r="N5" s="23">
+        <v>1</v>
+      </c>
+      <c r="O5" s="23">
+        <v>1</v>
+      </c>
+      <c r="P5" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>1</v>
+      </c>
+      <c r="R5" s="23">
+        <v>1</v>
+      </c>
+      <c r="S5" s="23">
+        <v>1</v>
+      </c>
+      <c r="T5" s="23">
+        <v>1</v>
+      </c>
+      <c r="U5" s="23">
+        <v>1</v>
+      </c>
+      <c r="V5" s="23">
+        <v>1</v>
+      </c>
+      <c r="W5" s="23">
         <v>1</v>
       </c>
     </row>
@@ -3423,7 +3622,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3499,82 +3698,83 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:D17"/>
+      <selection activeCell="C16" sqref="C16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="4" width="16.83203125" customWidth="1"/>
+    <col min="3" max="8" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="18">
-        <v>654000</v>
+        <v>653846.15384615387</v>
       </c>
       <c r="D2" s="18">
-        <v>108000</v>
+        <v>107692.3076923077</v>
       </c>
       <c r="E2" s="18">
-        <v>517000</v>
+        <v>310030.39513677813</v>
       </c>
       <c r="F2" s="18">
-        <v>33000</v>
+        <v>20060.790273556231</v>
       </c>
       <c r="H2" s="18">
-        <v>1311000</v>
+        <f>SUM(C2:F2)</f>
+        <v>1091629.646948796</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C3" s="19">
         <f>C2/$H2</f>
-        <v>0.4988558352402746</v>
+        <v>0.59896335325237204</v>
       </c>
       <c r="D3" s="19">
         <f t="shared" ref="D3:F3" si="0">D2/$H2</f>
-        <v>8.2379862700228831E-2</v>
+        <v>9.8652787594508337E-2</v>
       </c>
       <c r="E3" s="19">
         <f t="shared" si="0"/>
-        <v>0.39435545385202136</v>
+        <v>0.28400693953607914</v>
       </c>
       <c r="F3" s="19">
         <f t="shared" si="0"/>
-        <v>2.5171624713958809E-2</v>
+        <v>1.8376919617040414E-2</v>
       </c>
       <c r="H3" s="19">
         <f>SUM(C3:F3)</f>
-        <v>1.0007627765064837</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4" s="19">
         <f>C2/(C2+D2)</f>
-        <v>0.8582677165354331</v>
+        <v>0.85858585858585856</v>
       </c>
       <c r="D4" s="19">
         <f>1-C4</f>
-        <v>0.1417322834645669</v>
+        <v>0.14141414141414144</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
@@ -3589,13 +3789,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -3623,7 +3823,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8">
         <v>480</v>
@@ -3632,10 +3832,10 @@
         <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8">
         <v>13</v>
@@ -3664,7 +3864,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10">
         <v>0.85</v>
@@ -3733,21 +3933,21 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15">
         <v>0.02</v>
       </c>
       <c r="C15">
-        <f>$B15*C12</f>
-        <v>1.7171717171717171E-2</v>
+        <f>$B15*C11</f>
+        <v>1.0559006211180125E-2</v>
       </c>
       <c r="D15">
-        <f>$B15*D12</f>
-        <v>2.8282828282828287E-3</v>
+        <f t="shared" ref="D15:F15" si="2">$B15*D11</f>
+        <v>1.739130434782609E-3</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E15:F15" si="2">$B15*E11</f>
+        <f t="shared" si="2"/>
         <v>7.4534161490683237E-3</v>
       </c>
       <c r="F15">
@@ -3757,36 +3957,37 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="5">
+        <f>215000*0.1</f>
         <v>21500</v>
       </c>
       <c r="C16">
-        <f>B16*$C3</f>
-        <v>10725.400457665904</v>
+        <f>$B16*C3</f>
+        <v>12877.712094925999</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16:F16" si="3">C16*$C3</f>
-        <v>5350.4286035953482</v>
+        <f t="shared" ref="D16:F16" si="3">$B16*D3</f>
+        <v>2121.0349332819292</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>2669.0925299400137</v>
+        <v>6106.1492000257012</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>1331.4923833568032</v>
+        <v>395.10377176636888</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17">
         <f>B16*C4</f>
-        <v>18452.755905511811</v>
+        <v>18459.595959595958</v>
       </c>
       <c r="D17">
         <f>C16*D4</f>
-        <v>1520.1354979368996</v>
+        <v>1821.0905992824648</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Visualizations -- and fixed EB's portfolio's hydrogen
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio - Current Projects 1.29.2024.xlsx
+++ b/data/SJV Portfolio - Current Projects 1.29.2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F118EA7E-10F1-4E44-8A47-05F558FFB153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D6178C-2529-4545-8B57-113DAA49994B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="880" windowWidth="34000" windowHeight="17980" activeTab="2" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
   </bookViews>
@@ -1511,7 +1511,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1618,43 +1618,43 @@
         <v>66</v>
       </c>
       <c r="F2">
-        <f>$P2/11</f>
+        <f t="shared" ref="F2:F7" si="0">$P2/11</f>
         <v>1209.090909090909</v>
       </c>
       <c r="G2">
-        <f>$P2/11+F2</f>
+        <f t="shared" ref="G2:G7" si="1">$P2/11+F2</f>
         <v>2418.181818181818</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:O2" si="0">$P2/11+G2</f>
+        <f t="shared" ref="H2:O2" si="2">$P2/11+G2</f>
         <v>3627.272727272727</v>
       </c>
       <c r="I2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4836.363636363636</v>
       </c>
       <c r="J2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6045.454545454545</v>
       </c>
       <c r="K2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7254.545454545454</v>
       </c>
       <c r="L2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8463.636363636364</v>
       </c>
       <c r="M2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9672.7272727272721</v>
       </c>
       <c r="N2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10881.81818181818</v>
       </c>
       <c r="O2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>12090.909090909088</v>
       </c>
       <c r="P2">
@@ -1662,43 +1662,43 @@
         <v>13300</v>
       </c>
       <c r="Q2">
-        <f>$P2</f>
+        <f t="shared" ref="Q2:Q7" si="3">$P2</f>
         <v>13300</v>
       </c>
       <c r="R2">
-        <f t="shared" ref="R2:Z2" si="1">$P2</f>
+        <f t="shared" ref="R2:Z2" si="4">$P2</f>
         <v>13300</v>
       </c>
       <c r="S2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13300</v>
       </c>
       <c r="T2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13300</v>
       </c>
       <c r="U2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13300</v>
       </c>
       <c r="V2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13300</v>
       </c>
       <c r="W2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13300</v>
       </c>
       <c r="X2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13300</v>
       </c>
       <c r="Y2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13300</v>
       </c>
       <c r="Z2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13300</v>
       </c>
     </row>
@@ -1719,43 +1719,43 @@
         <v>66</v>
       </c>
       <c r="F3">
-        <f>$P3/11</f>
+        <f t="shared" si="0"/>
         <v>24.545454545454547</v>
       </c>
       <c r="G3">
-        <f>$P3/11+F3</f>
+        <f t="shared" si="1"/>
         <v>49.090909090909093</v>
       </c>
       <c r="H3">
-        <f>$P3/11+G3</f>
+        <f t="shared" ref="H3:O7" si="5">$P3/11+G3</f>
         <v>73.63636363636364</v>
       </c>
       <c r="I3">
-        <f>$P3/11+H3</f>
+        <f t="shared" si="5"/>
         <v>98.181818181818187</v>
       </c>
       <c r="J3">
-        <f>$P3/11+I3</f>
+        <f t="shared" si="5"/>
         <v>122.72727272727273</v>
       </c>
       <c r="K3">
-        <f>$P3/11+J3</f>
+        <f t="shared" si="5"/>
         <v>147.27272727272728</v>
       </c>
       <c r="L3">
-        <f>$P3/11+K3</f>
+        <f t="shared" si="5"/>
         <v>171.81818181818181</v>
       </c>
       <c r="M3">
-        <f>$P3/11+L3</f>
+        <f t="shared" si="5"/>
         <v>196.36363636363637</v>
       </c>
       <c r="N3">
-        <f>$P3/11+M3</f>
+        <f t="shared" si="5"/>
         <v>220.90909090909093</v>
       </c>
       <c r="O3">
-        <f>$P3/11+N3</f>
+        <f t="shared" si="5"/>
         <v>245.4545454545455</v>
       </c>
       <c r="P3">
@@ -1763,43 +1763,43 @@
         <v>270</v>
       </c>
       <c r="Q3">
-        <f>$P3</f>
+        <f t="shared" si="3"/>
         <v>270</v>
       </c>
       <c r="R3">
-        <f>$P3</f>
+        <f t="shared" ref="R3:Z7" si="6">$P3</f>
         <v>270</v>
       </c>
       <c r="S3">
-        <f>$P3</f>
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
       <c r="T3">
-        <f>$P3</f>
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
       <c r="U3">
-        <f>$P3</f>
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
       <c r="V3">
-        <f>$P3</f>
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
       <c r="W3">
-        <f>$P3</f>
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
       <c r="X3">
-        <f>$P3</f>
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
       <c r="Y3">
-        <f>$P3</f>
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
       <c r="Z3">
-        <f>$P3</f>
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
     </row>
@@ -1820,43 +1820,43 @@
         <v>66</v>
       </c>
       <c r="F4">
-        <f>$P4/11</f>
+        <f t="shared" si="0"/>
         <v>672.72727272727275</v>
       </c>
       <c r="G4">
-        <f>$P4/11+F4</f>
+        <f t="shared" si="1"/>
         <v>1345.4545454545455</v>
       </c>
       <c r="H4">
-        <f>$P4/11+G4</f>
+        <f t="shared" si="5"/>
         <v>2018.1818181818182</v>
       </c>
       <c r="I4">
-        <f>$P4/11+H4</f>
+        <f t="shared" si="5"/>
         <v>2690.909090909091</v>
       </c>
       <c r="J4">
-        <f>$P4/11+I4</f>
+        <f t="shared" si="5"/>
         <v>3363.636363636364</v>
       </c>
       <c r="K4">
-        <f>$P4/11+J4</f>
+        <f t="shared" si="5"/>
         <v>4036.3636363636369</v>
       </c>
       <c r="L4">
-        <f>$P4/11+K4</f>
+        <f t="shared" si="5"/>
         <v>4709.0909090909099</v>
       </c>
       <c r="M4">
-        <f>$P4/11+L4</f>
+        <f t="shared" si="5"/>
         <v>5381.8181818181829</v>
       </c>
       <c r="N4">
-        <f>$P4/11+M4</f>
+        <f t="shared" si="5"/>
         <v>6054.5454545454559</v>
       </c>
       <c r="O4">
-        <f>$P4/11+N4</f>
+        <f t="shared" si="5"/>
         <v>6727.2727272727288</v>
       </c>
       <c r="P4">
@@ -1864,43 +1864,43 @@
         <v>7400</v>
       </c>
       <c r="Q4">
-        <f>$P4</f>
+        <f t="shared" si="3"/>
         <v>7400</v>
       </c>
       <c r="R4">
-        <f>$P4</f>
+        <f t="shared" si="6"/>
         <v>7400</v>
       </c>
       <c r="S4">
-        <f>$P4</f>
+        <f t="shared" si="6"/>
         <v>7400</v>
       </c>
       <c r="T4">
-        <f>$P4</f>
+        <f t="shared" si="6"/>
         <v>7400</v>
       </c>
       <c r="U4">
-        <f>$P4</f>
+        <f t="shared" si="6"/>
         <v>7400</v>
       </c>
       <c r="V4">
-        <f>$P4</f>
+        <f t="shared" si="6"/>
         <v>7400</v>
       </c>
       <c r="W4">
-        <f>$P4</f>
+        <f t="shared" si="6"/>
         <v>7400</v>
       </c>
       <c r="X4">
-        <f>$P4</f>
+        <f t="shared" si="6"/>
         <v>7400</v>
       </c>
       <c r="Y4">
-        <f>$P4</f>
+        <f t="shared" si="6"/>
         <v>7400</v>
       </c>
       <c r="Z4">
-        <f>$P4</f>
+        <f t="shared" si="6"/>
         <v>7400</v>
       </c>
     </row>
@@ -1921,43 +1921,43 @@
         <v>66</v>
       </c>
       <c r="F5">
-        <f>$P5/11</f>
+        <f t="shared" si="0"/>
         <v>90.909090909090907</v>
       </c>
       <c r="G5">
-        <f>$P5/11+F5</f>
+        <f t="shared" si="1"/>
         <v>181.81818181818181</v>
       </c>
       <c r="H5">
-        <f>$P5/11+G5</f>
+        <f t="shared" si="5"/>
         <v>272.72727272727275</v>
       </c>
       <c r="I5">
-        <f>$P5/11+H5</f>
+        <f t="shared" si="5"/>
         <v>363.63636363636363</v>
       </c>
       <c r="J5">
-        <f>$P5/11+I5</f>
+        <f t="shared" si="5"/>
         <v>454.5454545454545</v>
       </c>
       <c r="K5">
-        <f>$P5/11+J5</f>
+        <f t="shared" si="5"/>
         <v>545.45454545454538</v>
       </c>
       <c r="L5">
-        <f>$P5/11+K5</f>
+        <f t="shared" si="5"/>
         <v>636.36363636363626</v>
       </c>
       <c r="M5">
-        <f>$P5/11+L5</f>
+        <f t="shared" si="5"/>
         <v>727.27272727272714</v>
       </c>
       <c r="N5">
-        <f>$P5/11+M5</f>
+        <f t="shared" si="5"/>
         <v>818.18181818181802</v>
       </c>
       <c r="O5">
-        <f>$P5/11+N5</f>
+        <f t="shared" si="5"/>
         <v>909.09090909090889</v>
       </c>
       <c r="P5">
@@ -1965,43 +1965,43 @@
         <v>1000</v>
       </c>
       <c r="Q5">
-        <f>$P5</f>
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
       <c r="R5">
-        <f>$P5</f>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="S5">
-        <f>$P5</f>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="T5">
-        <f>$P5</f>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="U5">
-        <f>$P5</f>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="V5">
-        <f>$P5</f>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="W5">
-        <f>$P5</f>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="X5">
-        <f>$P5</f>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="Y5">
-        <f>$P5</f>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="Z5">
-        <f>$P5</f>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
     </row>
@@ -2022,43 +2022,43 @@
         <v>66</v>
       </c>
       <c r="F6">
-        <f>$P6/11</f>
+        <f t="shared" si="0"/>
         <v>0.9599096555618295</v>
       </c>
       <c r="G6">
-        <f>$P6/11+F6</f>
+        <f t="shared" si="1"/>
         <v>1.919819311123659</v>
       </c>
       <c r="H6">
-        <f>$P6/11+G6</f>
+        <f t="shared" si="5"/>
         <v>2.8797289666854886</v>
       </c>
       <c r="I6">
-        <f>$P6/11+H6</f>
+        <f t="shared" si="5"/>
         <v>3.839638622247318</v>
       </c>
       <c r="J6">
-        <f>$P6/11+I6</f>
+        <f t="shared" si="5"/>
         <v>4.7995482778091478</v>
       </c>
       <c r="K6">
-        <f>$P6/11+J6</f>
+        <f t="shared" si="5"/>
         <v>5.7594579333709772</v>
       </c>
       <c r="L6">
-        <f>$P6/11+K6</f>
+        <f t="shared" si="5"/>
         <v>6.7193675889328066</v>
       </c>
       <c r="M6">
-        <f>$P6/11+L6</f>
+        <f t="shared" si="5"/>
         <v>7.679277244494636</v>
       </c>
       <c r="N6">
-        <f>$P6/11+M6</f>
+        <f t="shared" si="5"/>
         <v>8.6391869000564654</v>
       </c>
       <c r="O6">
-        <f>$P6/11+N6</f>
+        <f t="shared" si="5"/>
         <v>9.5990965556182957</v>
       </c>
       <c r="P6">
@@ -2066,43 +2066,43 @@
         <v>10.559006211180124</v>
       </c>
       <c r="Q6">
-        <f>$P6</f>
+        <f t="shared" si="3"/>
         <v>10.559006211180124</v>
       </c>
       <c r="R6">
-        <f>$P6</f>
+        <f t="shared" si="6"/>
         <v>10.559006211180124</v>
       </c>
       <c r="S6">
-        <f>$P6</f>
+        <f t="shared" si="6"/>
         <v>10.559006211180124</v>
       </c>
       <c r="T6">
-        <f>$P6</f>
+        <f t="shared" si="6"/>
         <v>10.559006211180124</v>
       </c>
       <c r="U6">
-        <f>$P6</f>
+        <f t="shared" si="6"/>
         <v>10.559006211180124</v>
       </c>
       <c r="V6">
-        <f>$P6</f>
+        <f t="shared" si="6"/>
         <v>10.559006211180124</v>
       </c>
       <c r="W6">
-        <f>$P6</f>
+        <f t="shared" si="6"/>
         <v>10.559006211180124</v>
       </c>
       <c r="X6">
-        <f>$P6</f>
+        <f t="shared" si="6"/>
         <v>10.559006211180124</v>
       </c>
       <c r="Y6">
-        <f>$P6</f>
+        <f t="shared" si="6"/>
         <v>10.559006211180124</v>
       </c>
       <c r="Z6">
-        <f>$P6</f>
+        <f t="shared" si="6"/>
         <v>10.559006211180124</v>
       </c>
     </row>
@@ -2123,43 +2123,43 @@
         <v>66</v>
       </c>
       <c r="F7">
-        <f>$P7/11</f>
+        <f t="shared" si="0"/>
         <v>0.15810276679841898</v>
       </c>
       <c r="G7">
-        <f>$P7/11+F7</f>
+        <f t="shared" si="1"/>
         <v>0.31620553359683795</v>
       </c>
       <c r="H7">
-        <f>$P7/11+G7</f>
+        <f t="shared" si="5"/>
         <v>0.47430830039525695</v>
       </c>
       <c r="I7">
-        <f>$P7/11+H7</f>
+        <f t="shared" si="5"/>
         <v>0.6324110671936759</v>
       </c>
       <c r="J7">
-        <f>$P7/11+I7</f>
+        <f t="shared" si="5"/>
         <v>0.79051383399209485</v>
       </c>
       <c r="K7">
-        <f>$P7/11+J7</f>
+        <f t="shared" si="5"/>
         <v>0.9486166007905138</v>
       </c>
       <c r="L7">
-        <f>$P7/11+K7</f>
+        <f t="shared" si="5"/>
         <v>1.1067193675889329</v>
       </c>
       <c r="M7">
-        <f>$P7/11+L7</f>
+        <f t="shared" si="5"/>
         <v>1.2648221343873518</v>
       </c>
       <c r="N7">
-        <f>$P7/11+M7</f>
+        <f t="shared" si="5"/>
         <v>1.4229249011857708</v>
       </c>
       <c r="O7">
-        <f>$P7/11+N7</f>
+        <f t="shared" si="5"/>
         <v>1.5810276679841897</v>
       </c>
       <c r="P7">
@@ -2167,43 +2167,43 @@
         <v>1.7391304347826089</v>
       </c>
       <c r="Q7">
-        <f>$P7</f>
+        <f t="shared" si="3"/>
         <v>1.7391304347826089</v>
       </c>
       <c r="R7">
-        <f>$P7</f>
+        <f t="shared" si="6"/>
         <v>1.7391304347826089</v>
       </c>
       <c r="S7">
-        <f>$P7</f>
+        <f t="shared" si="6"/>
         <v>1.7391304347826089</v>
       </c>
       <c r="T7">
-        <f>$P7</f>
+        <f t="shared" si="6"/>
         <v>1.7391304347826089</v>
       </c>
       <c r="U7">
-        <f>$P7</f>
+        <f t="shared" si="6"/>
         <v>1.7391304347826089</v>
       </c>
       <c r="V7">
-        <f>$P7</f>
+        <f t="shared" si="6"/>
         <v>1.7391304347826089</v>
       </c>
       <c r="W7">
-        <f>$P7</f>
+        <f t="shared" si="6"/>
         <v>1.7391304347826089</v>
       </c>
       <c r="X7">
-        <f>$P7</f>
+        <f t="shared" si="6"/>
         <v>1.7391304347826089</v>
       </c>
       <c r="Y7">
-        <f>$P7</f>
+        <f t="shared" si="6"/>
         <v>1.7391304347826089</v>
       </c>
       <c r="Z7">
-        <f>$P7</f>
+        <f t="shared" si="6"/>
         <v>1.7391304347826089</v>
       </c>
     </row>
@@ -2224,43 +2224,43 @@
         <v>66</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F9" si="2">$P8/11</f>
+        <f t="shared" ref="F8:F9" si="7">$P8/11</f>
         <v>0.67758328627893849</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:O9" si="3">$P8/11+F8</f>
+        <f t="shared" ref="G8:O9" si="8">$P8/11+F8</f>
         <v>1.355166572557877</v>
       </c>
       <c r="H8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2.0327498588368154</v>
       </c>
       <c r="I8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2.710333145115754</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.3879164313946926</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>4.0654997176736307</v>
       </c>
       <c r="L8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>4.7430830039525693</v>
       </c>
       <c r="M8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>5.4206662902315079</v>
       </c>
       <c r="N8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>6.0982495765104465</v>
       </c>
       <c r="O8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>6.7758328627893851</v>
       </c>
       <c r="P8">
@@ -2268,43 +2268,43 @@
         <v>7.4534161490683237</v>
       </c>
       <c r="Q8">
-        <f t="shared" ref="Q8:Z9" si="4">$P8</f>
+        <f t="shared" ref="Q8:Z9" si="9">$P8</f>
         <v>7.4534161490683237</v>
       </c>
       <c r="R8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>7.4534161490683237</v>
       </c>
       <c r="S8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>7.4534161490683237</v>
       </c>
       <c r="T8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>7.4534161490683237</v>
       </c>
       <c r="U8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>7.4534161490683237</v>
       </c>
       <c r="V8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>7.4534161490683237</v>
       </c>
       <c r="W8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>7.4534161490683237</v>
       </c>
       <c r="X8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>7.4534161490683237</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>7.4534161490683237</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>7.4534161490683237</v>
       </c>
     </row>
@@ -2325,43 +2325,43 @@
         <v>66</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2.258610954263128E-2</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>4.517221908526256E-2</v>
       </c>
       <c r="H9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>6.7758328627893841E-2</v>
       </c>
       <c r="I9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>9.0344438170525121E-2</v>
       </c>
       <c r="J9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.1129305477131564</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.13551665725578768</v>
       </c>
       <c r="L9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.15810276679841895</v>
       </c>
       <c r="M9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.18068887634105024</v>
       </c>
       <c r="N9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.20327498588368154</v>
       </c>
       <c r="O9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.22586109542631283</v>
       </c>
       <c r="P9">
@@ -2369,43 +2369,43 @@
         <v>0.2484472049689441</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.2484472049689441</v>
       </c>
       <c r="R9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.2484472049689441</v>
       </c>
       <c r="S9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.2484472049689441</v>
       </c>
       <c r="T9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.2484472049689441</v>
       </c>
       <c r="U9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.2484472049689441</v>
       </c>
       <c r="V9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.2484472049689441</v>
       </c>
       <c r="W9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.2484472049689441</v>
       </c>
       <c r="X9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.2484472049689441</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.2484472049689441</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.2484472049689441</v>
       </c>
     </row>
@@ -2430,39 +2430,39 @@
         <v>17590.909090909092</v>
       </c>
       <c r="G10">
-        <f>$P10/11+F10</f>
+        <f t="shared" ref="G10:O10" si="10">$P10/11+F10</f>
         <v>35181.818181818184</v>
       </c>
       <c r="H10">
-        <f>$P10/11+G10</f>
+        <f t="shared" si="10"/>
         <v>52772.727272727279</v>
       </c>
       <c r="I10">
-        <f>$P10/11+H10</f>
+        <f t="shared" si="10"/>
         <v>70363.636363636368</v>
       </c>
       <c r="J10">
-        <f>$P10/11+I10</f>
+        <f t="shared" si="10"/>
         <v>87954.545454545456</v>
       </c>
       <c r="K10">
-        <f>$P10/11+J10</f>
+        <f t="shared" si="10"/>
         <v>105545.45454545454</v>
       </c>
       <c r="L10">
-        <f>$P10/11+K10</f>
+        <f t="shared" si="10"/>
         <v>123136.36363636363</v>
       </c>
       <c r="M10">
-        <f>$P10/11+L10</f>
+        <f t="shared" si="10"/>
         <v>140727.27272727274</v>
       </c>
       <c r="N10">
-        <f>$P10/11+M10</f>
+        <f t="shared" si="10"/>
         <v>158318.18181818182</v>
       </c>
       <c r="O10">
-        <f>$P10/11+N10</f>
+        <f t="shared" si="10"/>
         <v>175909.09090909091</v>
       </c>
       <c r="P10" s="24">
@@ -2470,43 +2470,43 @@
         <v>193500</v>
       </c>
       <c r="Q10">
-        <f>$P10</f>
+        <f t="shared" ref="Q10:Z12" si="11">$P10</f>
         <v>193500</v>
       </c>
       <c r="R10">
-        <f>$P10</f>
+        <f t="shared" si="11"/>
         <v>193500</v>
       </c>
       <c r="S10">
-        <f>$P10</f>
+        <f t="shared" si="11"/>
         <v>193500</v>
       </c>
       <c r="T10">
-        <f>$P10</f>
+        <f t="shared" si="11"/>
         <v>193500</v>
       </c>
       <c r="U10">
-        <f>$P10</f>
+        <f t="shared" si="11"/>
         <v>193500</v>
       </c>
       <c r="V10">
-        <f>$P10</f>
+        <f t="shared" si="11"/>
         <v>193500</v>
       </c>
       <c r="W10">
-        <f>$P10</f>
+        <f t="shared" si="11"/>
         <v>193500</v>
       </c>
       <c r="X10">
-        <f>$P10</f>
+        <f t="shared" si="11"/>
         <v>193500</v>
       </c>
       <c r="Y10">
-        <f>$P10</f>
+        <f t="shared" si="11"/>
         <v>193500</v>
       </c>
       <c r="Z10">
-        <f>$P10</f>
+        <f t="shared" si="11"/>
         <v>193500</v>
       </c>
     </row>
@@ -2531,39 +2531,39 @@
         <v>1000</v>
       </c>
       <c r="G11">
-        <f>$P11/11+F11</f>
+        <f t="shared" ref="G11:O11" si="12">$P11/11+F11</f>
         <v>2000</v>
       </c>
       <c r="H11">
-        <f>$P11/11+G11</f>
+        <f t="shared" si="12"/>
         <v>3000</v>
       </c>
       <c r="I11">
-        <f>$P11/11+H11</f>
+        <f t="shared" si="12"/>
         <v>4000</v>
       </c>
       <c r="J11">
-        <f>$P11/11+I11</f>
+        <f t="shared" si="12"/>
         <v>5000</v>
       </c>
       <c r="K11">
-        <f>$P11/11+J11</f>
+        <f t="shared" si="12"/>
         <v>6000</v>
       </c>
       <c r="L11">
-        <f>$P11/11+K11</f>
+        <f t="shared" si="12"/>
         <v>7000</v>
       </c>
       <c r="M11">
-        <f>$P11/11+L11</f>
+        <f t="shared" si="12"/>
         <v>8000</v>
       </c>
       <c r="N11">
-        <f>$P11/11+M11</f>
+        <f t="shared" si="12"/>
         <v>9000</v>
       </c>
       <c r="O11">
-        <f>$P11/11+N11</f>
+        <f t="shared" si="12"/>
         <v>10000</v>
       </c>
       <c r="P11" s="24">
@@ -2571,43 +2571,43 @@
         <v>11000</v>
       </c>
       <c r="Q11">
-        <f>$P11</f>
+        <f t="shared" si="11"/>
         <v>11000</v>
       </c>
       <c r="R11">
-        <f>$P11</f>
+        <f t="shared" si="11"/>
         <v>11000</v>
       </c>
       <c r="S11">
-        <f>$P11</f>
+        <f t="shared" si="11"/>
         <v>11000</v>
       </c>
       <c r="T11">
-        <f>$P11</f>
+        <f t="shared" si="11"/>
         <v>11000</v>
       </c>
       <c r="U11">
-        <f>$P11</f>
+        <f t="shared" si="11"/>
         <v>11000</v>
       </c>
       <c r="V11">
-        <f>$P11</f>
+        <f t="shared" si="11"/>
         <v>11000</v>
       </c>
       <c r="W11">
-        <f>$P11</f>
+        <f t="shared" si="11"/>
         <v>11000</v>
       </c>
       <c r="X11">
-        <f>$P11</f>
+        <f t="shared" si="11"/>
         <v>11000</v>
       </c>
       <c r="Y11">
-        <f>$P11</f>
+        <f t="shared" si="11"/>
         <v>11000</v>
       </c>
       <c r="Z11">
-        <f>$P11</f>
+        <f t="shared" si="11"/>
         <v>11000</v>
       </c>
     </row>
@@ -2632,39 +2632,39 @@
         <v>1170.7010995387272</v>
       </c>
       <c r="G12">
-        <f>$P12/11+F12</f>
+        <f t="shared" ref="G12:O12" si="13">$P12/11+F12</f>
         <v>2341.4021990774545</v>
       </c>
       <c r="H12">
-        <f>$P12/11+G12</f>
+        <f t="shared" si="13"/>
         <v>3512.1032986161817</v>
       </c>
       <c r="I12">
-        <f>$P12/11+H12</f>
+        <f t="shared" si="13"/>
         <v>4682.804398154909</v>
       </c>
       <c r="J12">
-        <f>$P12/11+I12</f>
+        <f t="shared" si="13"/>
         <v>5853.5054976936362</v>
       </c>
       <c r="K12">
-        <f>$P12/11+J12</f>
+        <f t="shared" si="13"/>
         <v>7024.2065972323635</v>
       </c>
       <c r="L12">
-        <f>$P12/11+K12</f>
+        <f t="shared" si="13"/>
         <v>8194.9076967710898</v>
       </c>
       <c r="M12">
-        <f>$P12/11+L12</f>
+        <f t="shared" si="13"/>
         <v>9365.608796309818</v>
       </c>
       <c r="N12">
-        <f>$P12/11+M12</f>
+        <f t="shared" si="13"/>
         <v>10536.309895848546</v>
       </c>
       <c r="O12">
-        <f>$P12/11+N12</f>
+        <f t="shared" si="13"/>
         <v>11707.010995387274</v>
       </c>
       <c r="P12" s="24">
@@ -2672,43 +2672,43 @@
         <v>12877.712094925999</v>
       </c>
       <c r="Q12">
-        <f>$P12</f>
+        <f t="shared" si="11"/>
         <v>12877.712094925999</v>
       </c>
       <c r="R12">
-        <f>$P12</f>
+        <f t="shared" si="11"/>
         <v>12877.712094925999</v>
       </c>
       <c r="S12">
-        <f>$P12</f>
+        <f t="shared" si="11"/>
         <v>12877.712094925999</v>
       </c>
       <c r="T12">
-        <f>$P12</f>
+        <f t="shared" si="11"/>
         <v>12877.712094925999</v>
       </c>
       <c r="U12">
-        <f>$P12</f>
+        <f t="shared" si="11"/>
         <v>12877.712094925999</v>
       </c>
       <c r="V12">
-        <f>$P12</f>
+        <f t="shared" si="11"/>
         <v>12877.712094925999</v>
       </c>
       <c r="W12">
-        <f>$P12</f>
+        <f t="shared" si="11"/>
         <v>12877.712094925999</v>
       </c>
       <c r="X12">
-        <f>$P12</f>
+        <f t="shared" si="11"/>
         <v>12877.712094925999</v>
       </c>
       <c r="Y12">
-        <f>$P12</f>
+        <f t="shared" si="11"/>
         <v>12877.712094925999</v>
       </c>
       <c r="Z12">
-        <f>$P12</f>
+        <f t="shared" si="11"/>
         <v>12877.712094925999</v>
       </c>
     </row>
@@ -2737,35 +2737,35 @@
         <v>385.64271514216892</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13:O13" si="5">$P13/11+G13</f>
+        <f t="shared" ref="H13:O13" si="14">$P13/11+G13</f>
         <v>578.46407271325336</v>
       </c>
       <c r="I13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>771.28543028433785</v>
       </c>
       <c r="J13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>964.10678785542234</v>
       </c>
       <c r="K13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>1156.9281454265067</v>
       </c>
       <c r="L13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>1349.7495029975912</v>
       </c>
       <c r="M13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>1542.5708605686757</v>
       </c>
       <c r="N13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>1735.3922181397602</v>
       </c>
       <c r="O13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v>1928.2135757108447</v>
       </c>
       <c r="P13" s="24">
@@ -2777,39 +2777,39 @@
         <v>2121.0349332819292</v>
       </c>
       <c r="R13">
-        <f t="shared" ref="R13:Z13" si="6">$P13</f>
+        <f t="shared" ref="R13:Z13" si="15">$P13</f>
         <v>2121.0349332819292</v>
       </c>
       <c r="S13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2121.0349332819292</v>
       </c>
       <c r="T13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2121.0349332819292</v>
       </c>
       <c r="U13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2121.0349332819292</v>
       </c>
       <c r="V13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2121.0349332819292</v>
       </c>
       <c r="W13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2121.0349332819292</v>
       </c>
       <c r="X13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2121.0349332819292</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2121.0349332819292</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>2121.0349332819292</v>
       </c>
     </row>
@@ -2830,43 +2830,43 @@
         <v>72</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14:F15" si="7">$P14/11</f>
+        <f t="shared" ref="F14:F15" si="16">$P14/11</f>
         <v>555.10447272960926</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:O15" si="8">$P14/11+F14</f>
+        <f t="shared" ref="G14:O15" si="17">$P14/11+F14</f>
         <v>1110.2089454592185</v>
       </c>
       <c r="H14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>1665.3134181888277</v>
       </c>
       <c r="I14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>2220.417890918437</v>
       </c>
       <c r="J14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>2775.5223636480464</v>
       </c>
       <c r="K14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>3330.6268363776558</v>
       </c>
       <c r="L14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>3885.7313091072651</v>
       </c>
       <c r="M14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>4440.835781836874</v>
       </c>
       <c r="N14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>4995.9402545664834</v>
       </c>
       <c r="O14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>5551.0447272960928</v>
       </c>
       <c r="P14" s="24">
@@ -2874,43 +2874,43 @@
         <v>6106.1492000257012</v>
       </c>
       <c r="Q14">
-        <f t="shared" ref="Q14:Z15" si="9">$P14</f>
+        <f t="shared" ref="Q14:Z15" si="18">$P14</f>
         <v>6106.1492000257012</v>
       </c>
       <c r="R14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>6106.1492000257012</v>
       </c>
       <c r="S14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>6106.1492000257012</v>
       </c>
       <c r="T14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>6106.1492000257012</v>
       </c>
       <c r="U14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>6106.1492000257012</v>
       </c>
       <c r="V14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>6106.1492000257012</v>
       </c>
       <c r="W14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>6106.1492000257012</v>
       </c>
       <c r="X14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>6106.1492000257012</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>6106.1492000257012</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>6106.1492000257012</v>
       </c>
     </row>
@@ -2931,43 +2931,43 @@
         <v>72</v>
       </c>
       <c r="F15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>35.918524706033537</v>
       </c>
       <c r="G15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>71.837049412067074</v>
       </c>
       <c r="H15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>107.75557411810061</v>
       </c>
       <c r="I15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>143.67409882413415</v>
       </c>
       <c r="J15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>179.59262353016769</v>
       </c>
       <c r="K15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>215.51114823620122</v>
       </c>
       <c r="L15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>251.42967294223476</v>
       </c>
       <c r="M15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>287.3481976482683</v>
       </c>
       <c r="N15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>323.26672235430181</v>
       </c>
       <c r="O15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>359.18524706033531</v>
       </c>
       <c r="P15" s="24">
@@ -2975,43 +2975,43 @@
         <v>395.10377176636888</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>395.10377176636888</v>
       </c>
       <c r="R15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>395.10377176636888</v>
       </c>
       <c r="S15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>395.10377176636888</v>
       </c>
       <c r="T15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>395.10377176636888</v>
       </c>
       <c r="U15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>395.10377176636888</v>
       </c>
       <c r="V15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>395.10377176636888</v>
       </c>
       <c r="W15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>395.10377176636888</v>
       </c>
       <c r="X15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>395.10377176636888</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>395.10377176636888</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>395.10377176636888</v>
       </c>
     </row>
@@ -3085,7 +3085,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B20" t="s">

</xml_diff>